<commit_message>
Co-authored-by: seanbar2000 <seanbar2000@users.noreply.github.com> Co-authored-by: orenlan1 <orenlan1@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-06-19 22:34:44</t>
+          <t>2024-06-21 12:43:00</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>101.7737615657357</v>
+        <v>92.17482069321431</v>
       </c>
       <c r="C2" t="n">
         <v>10</v>
@@ -467,11 +467,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-06-19 22:34:46</t>
+          <t>2024-06-21 12:43:02</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>102.1028349010992</v>
+        <v>95.04422199178917</v>
       </c>
       <c r="C3" t="n">
         <v>15</v>
@@ -480,52 +480,117 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-06-19 22:34:48</t>
+          <t>2024-06-21 12:43:04</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>102.6440614597434</v>
+        <v>93.23202087367801</v>
       </c>
       <c r="C4" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-06-19 22:34:50</t>
+          <t>2024-06-21 12:43:06</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>102.5635139439226</v>
+        <v>88.48835411854395</v>
       </c>
       <c r="C5" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-06-19 22:34:52</t>
+          <t>2024-06-21 12:43:08</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>95.57392779672659</v>
+        <v>89.38206578331143</v>
       </c>
       <c r="C6" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-06-19 22:34:54</t>
+          <t>2024-06-21 12:43:10</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>85.35817535784287</v>
+        <v>87.6110812220857</v>
       </c>
       <c r="C7" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-06-21 12:43:12</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>87.74086381440483</v>
+      </c>
+      <c r="C8" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-06-21 12:43:14</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>90.20887101482903</v>
+      </c>
+      <c r="C9" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-06-21 12:43:16</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>92.64957610426052</v>
+      </c>
+      <c r="C10" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-06-21 12:43:18</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>91.07388210456324</v>
+      </c>
+      <c r="C11" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-06-21 12:43:20</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>89.36651516833891</v>
+      </c>
+      <c r="C12" t="n">
         <v>36</v>
       </c>
     </row>
@@ -540,7 +605,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,57 +630,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-06-19 22:34:52</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Truck and Car</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>134.13 and 73.74</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-06-19 22:34:53</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Car and Truck</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>103.30 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-06-19 22:34:54</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Car and Truck</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>94.44 and 122.00</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
little twiks and changes
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,144 +454,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-06-21 12:43:00</t>
+          <t>2024-07-26 11:57:23</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>92.17482069321431</v>
+        <v>99.00326479502259</v>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-06-21 12:43:02</t>
+          <t>2024-07-26 11:57:26</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>95.04422199178917</v>
+        <v>99.00326479502259</v>
       </c>
       <c r="C3" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-06-21 12:43:04</t>
+          <t>2024-07-26 11:57:28</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>93.23202087367801</v>
+        <v>99.00326479502259</v>
       </c>
       <c r="C4" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-06-21 12:43:06</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>88.48835411854395</v>
-      </c>
-      <c r="C5" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2024-06-21 12:43:08</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>89.38206578331143</v>
-      </c>
-      <c r="C6" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2024-06-21 12:43:10</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>87.6110812220857</v>
-      </c>
-      <c r="C7" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2024-06-21 12:43:12</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>87.74086381440483</v>
-      </c>
-      <c r="C8" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2024-06-21 12:43:14</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>90.20887101482903</v>
-      </c>
-      <c r="C9" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2024-06-21 12:43:16</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>92.64957610426052</v>
-      </c>
-      <c r="C10" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2024-06-21 12:43:18</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>91.07388210456324</v>
-      </c>
-      <c r="C11" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2024-06-21 12:43:20</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>89.36651516833891</v>
-      </c>
-      <c r="C12" t="n">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial thoughts for drive, make_next_desicion and get_all_harazds_around_vehicle
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,45 +449,6 @@
         <is>
           <t>Density</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-07-26 11:57:23</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>99.00326479502259</v>
-      </c>
-      <c r="C2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-07-26 11:57:26</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>99.00326479502259</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-07-26 11:57:28</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>99.00326479502259</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -501,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,6 +487,312 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:28</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>57.40 and 90.70</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:28</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>114.81 and 95.71</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:28</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>104.73 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:28</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>103.94 and 95.46</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:29</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>85.61 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:29</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>102.74 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:29</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>89.08 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:30</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>103.45 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:30</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>107.26 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:30</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>66.65 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:30</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>107.40 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:30</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>80.07 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:30</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>99.26 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:31</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>100.17 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:31</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>98.51 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:31</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>66.08 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:32</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>64.28 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-07-27 11:30:32</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>92.91 and 0.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
supposedly working field of view, started using Vehicle.drive()
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,75 +490,75 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:28</t>
+          <t>2024-07-28 23:35:13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Truck and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>57.40 and 90.70</t>
+          <t>44.52 and 95.53</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:28</t>
+          <t>2024-07-28 23:35:14</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>114.81 and 95.71</t>
+          <t>47.26 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:28</t>
+          <t>2024-07-28 23:35:15</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Truck and Car</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>104.73 and 0.00</t>
+          <t>70.57 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:28</t>
+          <t>2024-07-28 23:35:15</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>103.94 and 95.46</t>
+          <t>54.00 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:29</t>
+          <t>2024-07-28 23:35:16</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -568,48 +568,48 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>85.61 and 0.00</t>
+          <t>51.05 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:29</t>
+          <t>2024-07-28 23:35:16</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Truck and Car</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>102.74 and 0.00</t>
+          <t>84.49 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:29</t>
+          <t>2024-07-28 23:35:17</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>89.08 and 0.00</t>
+          <t>98.77 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:30</t>
+          <t>2024-07-28 23:35:18</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -619,31 +619,31 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>103.45 and 0.00</t>
+          <t>47.60 and 60.64</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:30</t>
+          <t>2024-07-28 23:35:18</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>107.26 and 0.00</t>
+          <t>78.71 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:30</t>
+          <t>2024-07-28 23:35:19</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -653,14 +653,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>66.65 and 0.00</t>
+          <t>47.18 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:30</t>
+          <t>2024-07-28 23:35:19</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -670,14 +670,14 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>107.40 and 0.00</t>
+          <t>55.21 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:30</t>
+          <t>2024-07-28 23:35:19</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -687,31 +687,31 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>80.07 and 0.00</t>
+          <t>45.45 and 57.43</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:30</t>
+          <t>2024-07-28 23:35:19</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Truck and Truck</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>99.26 and 0.00</t>
+          <t>87.63 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:31</t>
+          <t>2024-07-28 23:35:20</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -721,75 +721,1401 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>100.17 and 0.00</t>
+          <t>71.56 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:31</t>
+          <t>2024-07-28 23:35:20</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Truck and Car</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>98.51 and 0.00</t>
+          <t>47.84 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:31</t>
+          <t>2024-07-28 23:35:20</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Truck and Car</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>66.08 and 0.00</t>
+          <t>97.59 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:32</t>
+          <t>2024-07-28 23:35:21</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Car and Truck</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>64.28 and 0.00</t>
+          <t>51.44 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2024-07-27 11:30:32</t>
+          <t>2024-07-28 23:35:21</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>Truck and Truck</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>66.30 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:21</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>52.21 and 58.43</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:21</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>50.07 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>77.33 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>Car and Truck</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>92.91 and 0.00</t>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>105.19 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:22</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>77.65 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:22</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>48.36 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:22</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>50.99 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:22</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>110.07 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:22</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>120.81 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:23</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Truck and Truck</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>79.90 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:23</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>50.49 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:23</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>104.82 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:23</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>89.90 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:24</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>47.95 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:24</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>95.06 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:24</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>94.57 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:24</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>47.42 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:24</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>113.75 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:24</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>115.73 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:24</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>50.03 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:25</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>80.44 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:25</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>124.03 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:25</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>81.99 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:25</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>110.15 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:25</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>69.94 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:26</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>96.54 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:26</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>87.47 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:26</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>81.61 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:26</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>92.90 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:27</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>112.18 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:27</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>107.98 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:27</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>103.31 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:27</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>96.82 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:27</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>106.66 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:28</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>90.79 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:28</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>87.94 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:28</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>92.22 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:29</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>77.47 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:29</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>125.88 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:29</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>96.74 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:29</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>106.64 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:29</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>100.51 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:30</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>89.06 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:30</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>99.34 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:30</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>90.08 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:30</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>105.96 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:31</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>93.16 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:31</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>110.34 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:31</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>115.64 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:31</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>83.49 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:31</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>127.81 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:32</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>111.27 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:32</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>96.02 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:32</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>107.73 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:32</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>87.20 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:33</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>96.02 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:33</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>118.89 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:33</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>102.38 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:33</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>101.07 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:34</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>92.41 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:34</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>81.69 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:34</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>110.80 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:34</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>103.54 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:35</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>89.30 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:35</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>115.56 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:35</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>90.36 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:35</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>90.66 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:35</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>111.13 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:36</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>111.98 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:36</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>88.01 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:36</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>81.65 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:37</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Truck and Truck</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>83.69 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:37</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>112.41 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:37</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>82.90 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:37</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>95.13 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:37</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>105.24 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:38</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>96.49 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2024-07-28 23:35:38</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>102.29 and 0.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
start of lane-switching algorithm
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,214 @@
         <is>
           <t>Density</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:45:38</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>100.0804194481402</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:45:40</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>97.73670682793352</v>
+      </c>
+      <c r="C3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:45:42</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>97.31738825339654</v>
+      </c>
+      <c r="C4" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:45:44</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>95.23234230223129</v>
+      </c>
+      <c r="C5" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:45:46</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>92.6567857709139</v>
+      </c>
+      <c r="C6" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:45:48</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>89.3488440283692</v>
+      </c>
+      <c r="C7" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:45:50</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>89.14872053614005</v>
+      </c>
+      <c r="C8" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:45:52</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>86.01621069767486</v>
+      </c>
+      <c r="C9" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:45:54</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>82.38666017015372</v>
+      </c>
+      <c r="C10" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:45:56</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>79.62855465991544</v>
+      </c>
+      <c r="C11" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:45:58</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>78.35310442587</v>
+      </c>
+      <c r="C12" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:46:00</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>79.10140228330833</v>
+      </c>
+      <c r="C13" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:46:02</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>76.36352199368717</v>
+      </c>
+      <c r="C14" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:46:04</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>74.95296951464908</v>
+      </c>
+      <c r="C15" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:46:06</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>78.40997691535971</v>
+      </c>
+      <c r="C16" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:46:08</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>80.40935495769017</v>
+      </c>
+      <c r="C17" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -462,7 +670,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,6 +695,40 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:46:03</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>30.33 and 55.83</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-07-30 22:46:04</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>64.24 and 0.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
cleanups and more work on lane switching
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-07-30 22:45:38</t>
+          <t>2024-08-01 12:37:40</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100.0804194481402</v>
+        <v>94.23897003537142</v>
       </c>
       <c r="C2" t="n">
         <v>8</v>
@@ -467,11 +467,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-07-30 22:45:40</t>
+          <t>2024-08-01 12:37:42</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>97.73670682793352</v>
+        <v>94.17275958540921</v>
       </c>
       <c r="C3" t="n">
         <v>16</v>
@@ -480,183 +480,92 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-07-30 22:45:42</t>
+          <t>2024-08-01 12:37:44</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>97.31738825339654</v>
+        <v>75.30477324354547</v>
       </c>
       <c r="C4" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-07-30 22:45:44</t>
+          <t>2024-08-01 12:37:46</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>95.23234230223129</v>
+        <v>64.54746880472618</v>
       </c>
       <c r="C5" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-07-30 22:45:46</t>
+          <t>2024-08-01 12:37:48</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92.6567857709139</v>
+        <v>51.6774092598811</v>
       </c>
       <c r="C6" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-07-30 22:45:48</t>
+          <t>2024-08-01 12:37:50</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>89.3488440283692</v>
+        <v>43.59545398424419</v>
       </c>
       <c r="C7" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-07-30 22:45:50</t>
+          <t>2024-08-01 12:37:52</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>89.14872053614005</v>
+        <v>36.5299700089092</v>
       </c>
       <c r="C8" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-07-30 22:45:52</t>
+          <t>2024-08-01 12:37:54</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>86.01621069767486</v>
+        <v>28.37919823182034</v>
       </c>
       <c r="C9" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-07-30 22:45:54</t>
+          <t>2024-08-01 12:37:56</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>82.38666017015372</v>
+        <v>22.26924060751913</v>
       </c>
       <c r="C10" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2024-07-30 22:45:56</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>79.62855465991544</v>
-      </c>
-      <c r="C11" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2024-07-30 22:45:58</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>78.35310442587</v>
-      </c>
-      <c r="C12" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2024-07-30 22:46:00</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>79.10140228330833</v>
-      </c>
-      <c r="C13" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2024-07-30 22:46:02</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>76.36352199368717</v>
-      </c>
-      <c r="C14" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2024-07-30 22:46:04</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>74.95296951464908</v>
-      </c>
-      <c r="C15" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2024-07-30 22:46:06</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>78.40997691535971</v>
-      </c>
-      <c r="C16" t="n">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2024-07-30 22:46:08</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>80.40935495769017</v>
-      </c>
-      <c r="C17" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -670,7 +579,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -698,7 +607,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-07-30 22:46:03</t>
+          <t>2024-08-01 12:37:44</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -708,14 +617,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>30.33 and 55.83</t>
+          <t>61.98 and 88.71</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-07-30 22:46:04</t>
+          <t>2024-08-01 12:37:44</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -725,7 +634,228 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>64.24 and 0.00</t>
+          <t>91.53 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-08-01 12:37:46</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.00 and 85.79</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-08-01 12:37:46</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>78.59 and 76.66</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-08-01 12:37:47</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>88.74 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-01 12:37:48</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>11.65 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-08-01 12:37:48</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>50.96 and 71.65</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-08-01 12:37:48</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>42.46 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-08-01 12:37:49</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>56.47 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-08-01 12:37:50</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>54.49 and 88.75</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-08-01 12:37:52</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.00 and 95.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-01 12:37:54</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.00 and 37.35</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-08-01 12:37:54</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0.00 and 46.56</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-01 12:37:55</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>7.27 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-01 12:37:57</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>54.27 and 0.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
somewhat working lane switching
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:40</t>
+          <t>2024-08-01 14:38:36</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>94.23897003537142</v>
+        <v>99.63962434601845</v>
       </c>
       <c r="C2" t="n">
         <v>8</v>
@@ -467,11 +467,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:42</t>
+          <t>2024-08-01 14:38:38</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>94.17275958540921</v>
+        <v>94.1239588734572</v>
       </c>
       <c r="C3" t="n">
         <v>16</v>
@@ -480,24 +480,24 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:44</t>
+          <t>2024-08-01 14:38:40</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>75.30477324354547</v>
+        <v>93.99338058734503</v>
       </c>
       <c r="C4" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:46</t>
+          <t>2024-08-01 14:38:42</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>64.54746880472618</v>
+        <v>92.9068630843538</v>
       </c>
       <c r="C5" t="n">
         <v>29</v>
@@ -506,66 +506,950 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:48</t>
+          <t>2024-08-01 14:38:44</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>51.6774092598811</v>
+        <v>91.09677477077619</v>
       </c>
       <c r="C6" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:50</t>
+          <t>2024-08-01 14:38:46</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>43.59545398424419</v>
+        <v>87.61478121144819</v>
       </c>
       <c r="C7" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:52</t>
+          <t>2024-08-01 14:38:48</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>36.5299700089092</v>
+        <v>90.90032766676555</v>
       </c>
       <c r="C8" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:54</t>
+          <t>2024-08-01 14:38:50</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>28.37919823182034</v>
+        <v>93.96696935863731</v>
       </c>
       <c r="C9" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:56</t>
+          <t>2024-08-01 14:38:52</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>22.26924060751913</v>
+        <v>92.75154441985644</v>
       </c>
       <c r="C10" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:38:54</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>94.79467075765214</v>
+      </c>
+      <c r="C11" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:38:56</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>93.26176871509648</v>
+      </c>
+      <c r="C12" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:38:58</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>92.77097316453455</v>
+      </c>
+      <c r="C13" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:00</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>91.27731138960397</v>
+      </c>
+      <c r="C14" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:02</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>91.75831846087792</v>
+      </c>
+      <c r="C15" t="n">
         <v>37</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:04</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>90.36598263460624</v>
+      </c>
+      <c r="C16" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:06</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>85.466104151707</v>
+      </c>
+      <c r="C17" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:08</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>83.94980764496104</v>
+      </c>
+      <c r="C18" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:10</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>83.04693978334386</v>
+      </c>
+      <c r="C19" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:12</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>84.00339765145657</v>
+      </c>
+      <c r="C20" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:14</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>87.72918140743302</v>
+      </c>
+      <c r="C21" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:16</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>85.32039607716204</v>
+      </c>
+      <c r="C22" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:18</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>88.0328737741916</v>
+      </c>
+      <c r="C23" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:20</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>88.36889718323201</v>
+      </c>
+      <c r="C24" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:22</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>90.27987715975632</v>
+      </c>
+      <c r="C25" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:24</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>93.11118222548862</v>
+      </c>
+      <c r="C26" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:26</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>90.61121137302374</v>
+      </c>
+      <c r="C27" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:28</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>92.27165352451701</v>
+      </c>
+      <c r="C28" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:30</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>89.84864035497743</v>
+      </c>
+      <c r="C29" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:32</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>90.68668463037534</v>
+      </c>
+      <c r="C30" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:34</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>90.91028291327493</v>
+      </c>
+      <c r="C31" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:36</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>88.84505844856974</v>
+      </c>
+      <c r="C32" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:38</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>91.27190221137501</v>
+      </c>
+      <c r="C33" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:40</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>88.63169657768859</v>
+      </c>
+      <c r="C34" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:42</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>84.99043460955967</v>
+      </c>
+      <c r="C35" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:44</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>86.69794582695847</v>
+      </c>
+      <c r="C36" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:46</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>87.89581445854949</v>
+      </c>
+      <c r="C37" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:48</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>87.83128808597196</v>
+      </c>
+      <c r="C38" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:50</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>87.46069254209365</v>
+      </c>
+      <c r="C39" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:52</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>86.91259744793325</v>
+      </c>
+      <c r="C40" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:54</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>87.92061565754298</v>
+      </c>
+      <c r="C41" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:56</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>89.49991927254833</v>
+      </c>
+      <c r="C42" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:39:58</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>89.27883757046339</v>
+      </c>
+      <c r="C43" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:00</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>90.39604069749599</v>
+      </c>
+      <c r="C44" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:02</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>90.32513001741538</v>
+      </c>
+      <c r="C45" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:04</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>86.97382515425564</v>
+      </c>
+      <c r="C46" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:06</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>88.56965991870638</v>
+      </c>
+      <c r="C47" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:08</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>88.25541047755812</v>
+      </c>
+      <c r="C48" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:10</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>88.94836978626194</v>
+      </c>
+      <c r="C49" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:13</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>86.96927682479071</v>
+      </c>
+      <c r="C50" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:15</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>86.17325237660853</v>
+      </c>
+      <c r="C51" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:17</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>89.12631556009913</v>
+      </c>
+      <c r="C52" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:19</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>88.61861881082778</v>
+      </c>
+      <c r="C53" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:21</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>87.87037361539033</v>
+      </c>
+      <c r="C54" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:23</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>92.04476640863834</v>
+      </c>
+      <c r="C55" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:25</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>89.85359862550263</v>
+      </c>
+      <c r="C56" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:27</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>91.79749376205937</v>
+      </c>
+      <c r="C57" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:29</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>90.88539477491199</v>
+      </c>
+      <c r="C58" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:31</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>93.37784777714549</v>
+      </c>
+      <c r="C59" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:33</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>88.25378930939736</v>
+      </c>
+      <c r="C60" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:35</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>88.65880261989481</v>
+      </c>
+      <c r="C61" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:37</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>87.36875373216657</v>
+      </c>
+      <c r="C62" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:39</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>81.90804925152362</v>
+      </c>
+      <c r="C63" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:41</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>78.1398673581229</v>
+      </c>
+      <c r="C64" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:43</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>69.85164277060836</v>
+      </c>
+      <c r="C65" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:45</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>71.04467537968392</v>
+      </c>
+      <c r="C66" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:47</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>67.3017886118719</v>
+      </c>
+      <c r="C67" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:49</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>62.57681425621418</v>
+      </c>
+      <c r="C68" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:51</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>60.19473045491458</v>
+      </c>
+      <c r="C69" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:53</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>60.99033213409332</v>
+      </c>
+      <c r="C70" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:55</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>58.50962432064123</v>
+      </c>
+      <c r="C71" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:57</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>53.86950790632879</v>
+      </c>
+      <c r="C72" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:40:59</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>55.82157628782896</v>
+      </c>
+      <c r="C73" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:41:01</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>55.60703691479848</v>
+      </c>
+      <c r="C74" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:41:03</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>54.79521199242265</v>
+      </c>
+      <c r="C75" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:41:05</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>52.51591077046029</v>
+      </c>
+      <c r="C76" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:41:07</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>56.12128206149486</v>
+      </c>
+      <c r="C77" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2024-08-01 14:41:09</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>56.0877555455687</v>
+      </c>
+      <c r="C78" t="n">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -579,7 +1463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,7 +1491,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:44</t>
+          <t>2024-08-01 14:40:39</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -617,14 +1501,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>61.98 and 88.71</t>
+          <t>2.87 and 64.43</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:44</t>
+          <t>2024-08-01 14:40:41</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -634,48 +1518,48 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>91.53 and 0.00</t>
+          <t>15.12 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:46</t>
+          <t>2024-08-01 14:40:41</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Car and Truck</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.00 and 85.79</t>
+          <t>46.38 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:46</t>
+          <t>2024-08-01 14:40:42</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Car and Truck</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>78.59 and 76.66</t>
+          <t>46.50 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:47</t>
+          <t>2024-08-01 14:40:43</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -685,177 +1569,58 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>88.74 and 0.00</t>
+          <t>65.76 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:48</t>
+          <t>2024-08-01 14:40:46</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Car and Truck</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>11.65 and 0.00</t>
+          <t>58.30 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:48</t>
+          <t>2024-08-01 14:40:47</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>50.96 and 71.65</t>
+          <t>0.00 and 37.97</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-08-01 12:37:48</t>
+          <t>2024-08-01 14:40:48</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>42.46 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2024-08-01 12:37:49</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>56.47 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2024-08-01 12:37:50</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>54.49 and 88.75</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2024-08-01 12:37:52</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>0.00 and 95.16</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2024-08-01 12:37:54</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>0.00 and 37.35</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2024-08-01 12:37:54</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>0.00 and 46.56</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2024-08-01 12:37:55</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>7.27 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2024-08-01 12:37:57</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>54.27 and 0.00</t>
+          <t>47.72 and 35.35</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
work on getting rid of switching lanes constantly
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-01 14:38:36</t>
+          <t>2024-08-01 23:38:04</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>99.63962434601845</v>
+        <v>91.4205680931119</v>
       </c>
       <c r="C2" t="n">
         <v>8</v>
@@ -467,102 +467,102 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-01 14:38:38</t>
+          <t>2024-08-01 23:38:06</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>94.1239588734572</v>
+        <v>88.74962667708041</v>
       </c>
       <c r="C3" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-01 14:38:40</t>
+          <t>2024-08-01 23:38:08</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>93.99338058734503</v>
+        <v>87.85429370935688</v>
       </c>
       <c r="C4" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-01 14:38:42</t>
+          <t>2024-08-01 23:38:10</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>92.9068630843538</v>
+        <v>90.86957256735271</v>
       </c>
       <c r="C5" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-01 14:38:44</t>
+          <t>2024-08-01 23:38:12</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>91.09677477077619</v>
+        <v>90.57737370162057</v>
       </c>
       <c r="C6" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-01 14:38:46</t>
+          <t>2024-08-01 23:38:14</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>87.61478121144819</v>
+        <v>89.41232255424354</v>
       </c>
       <c r="C7" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-08-01 14:38:48</t>
+          <t>2024-08-01 23:38:16</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>90.90032766676555</v>
+        <v>87.7830534781564</v>
       </c>
       <c r="C8" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-08-01 14:38:50</t>
+          <t>2024-08-01 23:38:18</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>93.96696935863731</v>
+        <v>87.41874851047552</v>
       </c>
       <c r="C9" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-08-01 14:38:52</t>
+          <t>2024-08-01 23:38:20</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>92.75154441985644</v>
+        <v>87.82659129924576</v>
       </c>
       <c r="C10" t="n">
         <v>39</v>
@@ -571,115 +571,115 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-08-01 14:38:54</t>
+          <t>2024-08-01 23:38:22</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>94.79467075765214</v>
+        <v>84.9634604477847</v>
       </c>
       <c r="C11" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-08-01 14:38:56</t>
+          <t>2024-08-01 23:38:24</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>93.26176871509648</v>
+        <v>84.71894660050089</v>
       </c>
       <c r="C12" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2024-08-01 14:38:58</t>
+          <t>2024-08-01 23:38:26</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>92.77097316453455</v>
+        <v>83.16940000186695</v>
       </c>
       <c r="C13" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:00</t>
+          <t>2024-08-01 23:38:28</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>91.27731138960397</v>
+        <v>84.47715599124989</v>
       </c>
       <c r="C14" t="n">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:02</t>
+          <t>2024-08-01 23:38:30</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>91.75831846087792</v>
+        <v>86.35074453200711</v>
       </c>
       <c r="C15" t="n">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:04</t>
+          <t>2024-08-01 23:38:32</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>90.36598263460624</v>
+        <v>89.00227941581667</v>
       </c>
       <c r="C16" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:06</t>
+          <t>2024-08-01 23:38:34</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>85.466104151707</v>
+        <v>91.23013116808508</v>
       </c>
       <c r="C17" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:08</t>
+          <t>2024-08-01 23:38:36</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>83.94980764496104</v>
+        <v>90.63300056977803</v>
       </c>
       <c r="C18" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:10</t>
+          <t>2024-08-01 23:38:38</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>83.04693978334386</v>
+        <v>87.6005660558649</v>
       </c>
       <c r="C19" t="n">
         <v>44</v>
@@ -688,63 +688,63 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:12</t>
+          <t>2024-08-01 23:38:40</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>84.00339765145657</v>
+        <v>89.90122398956612</v>
       </c>
       <c r="C20" t="n">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:14</t>
+          <t>2024-08-01 23:38:42</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>87.72918140743302</v>
+        <v>91.41992887055029</v>
       </c>
       <c r="C21" t="n">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:16</t>
+          <t>2024-08-01 23:38:44</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>85.32039607716204</v>
+        <v>92.65350835830715</v>
       </c>
       <c r="C22" t="n">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:18</t>
+          <t>2024-08-01 23:38:46</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>88.0328737741916</v>
+        <v>90.84479605778301</v>
       </c>
       <c r="C23" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:20</t>
+          <t>2024-08-01 23:38:48</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>88.36889718323201</v>
+        <v>88.99355930112117</v>
       </c>
       <c r="C24" t="n">
         <v>39</v>
@@ -753,141 +753,141 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:22</t>
+          <t>2024-08-01 23:38:50</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>90.27987715975632</v>
+        <v>90.86093611113014</v>
       </c>
       <c r="C25" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:24</t>
+          <t>2024-08-01 23:38:52</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>93.11118222548862</v>
+        <v>89.68750251088673</v>
       </c>
       <c r="C26" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:26</t>
+          <t>2024-08-01 23:38:54</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>90.61121137302374</v>
+        <v>91.52159424810495</v>
       </c>
       <c r="C27" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:28</t>
+          <t>2024-08-01 23:38:56</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>92.27165352451701</v>
+        <v>90.6174946117838</v>
       </c>
       <c r="C28" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:30</t>
+          <t>2024-08-01 23:38:58</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>89.84864035497743</v>
+        <v>89.59019823992998</v>
       </c>
       <c r="C29" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:32</t>
+          <t>2024-08-01 23:39:00</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>90.68668463037534</v>
+        <v>87.48098787903095</v>
       </c>
       <c r="C30" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:34</t>
+          <t>2024-08-01 23:39:02</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>90.91028291327493</v>
+        <v>87.65826965764958</v>
       </c>
       <c r="C31" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:36</t>
+          <t>2024-08-01 23:39:04</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>88.84505844856974</v>
+        <v>87.48385949086152</v>
       </c>
       <c r="C32" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:38</t>
+          <t>2024-08-01 23:39:06</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>91.27190221137501</v>
+        <v>86.45793031711911</v>
       </c>
       <c r="C33" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:40</t>
+          <t>2024-08-01 23:39:08</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>88.63169657768859</v>
+        <v>85.31379392362322</v>
       </c>
       <c r="C34" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:42</t>
+          <t>2024-08-01 23:39:10</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>84.99043460955967</v>
+        <v>85.989617598244</v>
       </c>
       <c r="C35" t="n">
         <v>41</v>
@@ -896,297 +896,297 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:44</t>
+          <t>2024-08-01 23:39:12</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>86.69794582695847</v>
+        <v>89.08432746547685</v>
       </c>
       <c r="C36" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:46</t>
+          <t>2024-08-01 23:39:14</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>87.89581445854949</v>
+        <v>87.55954036893198</v>
       </c>
       <c r="C37" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:48</t>
+          <t>2024-08-01 23:39:16</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>87.83128808597196</v>
+        <v>88.33345401621068</v>
       </c>
       <c r="C38" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:50</t>
+          <t>2024-08-01 23:39:18</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>87.46069254209365</v>
+        <v>90.90893664827134</v>
       </c>
       <c r="C39" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:52</t>
+          <t>2024-08-01 23:39:20</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>86.91259744793325</v>
+        <v>89.63271839597333</v>
       </c>
       <c r="C40" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:54</t>
+          <t>2024-08-01 23:39:22</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>87.92061565754298</v>
+        <v>91.24267812117257</v>
       </c>
       <c r="C41" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:56</t>
+          <t>2024-08-01 23:39:24</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>89.49991927254833</v>
+        <v>90.07613559613324</v>
       </c>
       <c r="C42" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2024-08-01 14:39:58</t>
+          <t>2024-08-01 23:39:26</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>89.27883757046339</v>
+        <v>91.58304430970378</v>
       </c>
       <c r="C43" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:00</t>
+          <t>2024-08-01 23:39:28</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>90.39604069749599</v>
+        <v>88.90335660286357</v>
       </c>
       <c r="C44" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:02</t>
+          <t>2024-08-01 23:39:30</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>90.32513001741538</v>
+        <v>86.127985856659</v>
       </c>
       <c r="C45" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:04</t>
+          <t>2024-08-01 23:39:32</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>86.97382515425564</v>
+        <v>85.00691848859337</v>
       </c>
       <c r="C46" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:06</t>
+          <t>2024-08-01 23:39:34</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>88.56965991870638</v>
+        <v>81.6838367226961</v>
       </c>
       <c r="C47" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:08</t>
+          <t>2024-08-01 23:39:36</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>88.25541047755812</v>
+        <v>80.39913349204038</v>
       </c>
       <c r="C48" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:10</t>
+          <t>2024-08-01 23:39:38</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>88.94836978626194</v>
+        <v>75.79337961914223</v>
       </c>
       <c r="C49" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:13</t>
+          <t>2024-08-01 23:39:40</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>86.96927682479071</v>
+        <v>78.0389623374069</v>
       </c>
       <c r="C50" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:15</t>
+          <t>2024-08-01 23:39:42</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>86.17325237660853</v>
+        <v>74.08394014752675</v>
       </c>
       <c r="C51" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:17</t>
+          <t>2024-08-01 23:39:44</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>89.12631556009913</v>
+        <v>73.16852488387315</v>
       </c>
       <c r="C52" t="n">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:19</t>
+          <t>2024-08-01 23:39:46</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>88.61861881082778</v>
+        <v>68.90259061136622</v>
       </c>
       <c r="C53" t="n">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:21</t>
+          <t>2024-08-01 23:39:48</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>87.87037361539033</v>
+        <v>71.56448459543594</v>
       </c>
       <c r="C54" t="n">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:23</t>
+          <t>2024-08-01 23:39:50</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>92.04476640863834</v>
+        <v>67.81097795170474</v>
       </c>
       <c r="C55" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:25</t>
+          <t>2024-08-01 23:39:52</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>89.85359862550263</v>
+        <v>68.13598788593448</v>
       </c>
       <c r="C56" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:27</t>
+          <t>2024-08-01 23:39:54</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>91.79749376205937</v>
+        <v>71.16600928558584</v>
       </c>
       <c r="C57" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:29</t>
+          <t>2024-08-01 23:39:56</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>90.88539477491199</v>
+        <v>68.28653754691052</v>
       </c>
       <c r="C58" t="n">
         <v>40</v>
@@ -1195,261 +1195,40 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:31</t>
+          <t>2024-08-01 23:39:58</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>93.37784777714549</v>
+        <v>72.41563115198697</v>
       </c>
       <c r="C59" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:33</t>
+          <t>2024-08-01 23:40:00</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>88.25378930939736</v>
+        <v>78.45094729436897</v>
       </c>
       <c r="C60" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:35</t>
+          <t>2024-08-01 23:40:02</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>88.65880261989481</v>
+        <v>76.55504925266138</v>
       </c>
       <c r="C61" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:37</t>
-        </is>
-      </c>
-      <c r="B62" t="n">
-        <v>87.36875373216657</v>
-      </c>
-      <c r="C62" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:39</t>
-        </is>
-      </c>
-      <c r="B63" t="n">
-        <v>81.90804925152362</v>
-      </c>
-      <c r="C63" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:41</t>
-        </is>
-      </c>
-      <c r="B64" t="n">
-        <v>78.1398673581229</v>
-      </c>
-      <c r="C64" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:43</t>
-        </is>
-      </c>
-      <c r="B65" t="n">
-        <v>69.85164277060836</v>
-      </c>
-      <c r="C65" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:45</t>
-        </is>
-      </c>
-      <c r="B66" t="n">
-        <v>71.04467537968392</v>
-      </c>
-      <c r="C66" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:47</t>
-        </is>
-      </c>
-      <c r="B67" t="n">
-        <v>67.3017886118719</v>
-      </c>
-      <c r="C67" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:49</t>
-        </is>
-      </c>
-      <c r="B68" t="n">
-        <v>62.57681425621418</v>
-      </c>
-      <c r="C68" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:51</t>
-        </is>
-      </c>
-      <c r="B69" t="n">
-        <v>60.19473045491458</v>
-      </c>
-      <c r="C69" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:53</t>
-        </is>
-      </c>
-      <c r="B70" t="n">
-        <v>60.99033213409332</v>
-      </c>
-      <c r="C70" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:55</t>
-        </is>
-      </c>
-      <c r="B71" t="n">
-        <v>58.50962432064123</v>
-      </c>
-      <c r="C71" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:57</t>
-        </is>
-      </c>
-      <c r="B72" t="n">
-        <v>53.86950790632879</v>
-      </c>
-      <c r="C72" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:59</t>
-        </is>
-      </c>
-      <c r="B73" t="n">
-        <v>55.82157628782896</v>
-      </c>
-      <c r="C73" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:41:01</t>
-        </is>
-      </c>
-      <c r="B74" t="n">
-        <v>55.60703691479848</v>
-      </c>
-      <c r="C74" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:41:03</t>
-        </is>
-      </c>
-      <c r="B75" t="n">
-        <v>54.79521199242265</v>
-      </c>
-      <c r="C75" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:41:05</t>
-        </is>
-      </c>
-      <c r="B76" t="n">
-        <v>52.51591077046029</v>
-      </c>
-      <c r="C76" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:41:07</t>
-        </is>
-      </c>
-      <c r="B77" t="n">
-        <v>56.12128206149486</v>
-      </c>
-      <c r="C77" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:41:09</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>56.0877555455687</v>
-      </c>
-      <c r="C78" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1463,7 +1242,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1491,24 +1270,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:39</t>
+          <t>2024-08-01 23:39:35</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2.87 and 64.43</t>
+          <t>37.06 and 2.16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:41</t>
+          <t>2024-08-01 23:39:36</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1518,14 +1297,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>15.12 and 0.00</t>
+          <t>35.43 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-01 14:40:41</t>
+          <t>2024-08-01 23:39:37</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1535,92 +1314,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>46.38 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:42</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>46.50 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:43</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>65.76 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:46</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>58.30 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:47</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Car and Truck</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0.00 and 37.97</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2024-08-01 14:40:48</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Car and Truck</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>47.72 and 35.35</t>
+          <t>25.29 and 0.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
smooth-ish lane swith, need to polish it add more stuff
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-01 16:33:55</t>
+          <t>2024-08-02 00:47:11</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>101.079600233979</v>
+        <v>98.03449780950287</v>
       </c>
       <c r="C2" t="n">
         <v>8</v>
@@ -467,11 +467,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-01 16:33:57</t>
+          <t>2024-08-02 00:47:13</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>99.18532196965744</v>
+        <v>92.86859255648324</v>
       </c>
       <c r="C3" t="n">
         <v>16</v>
@@ -480,50 +480,50 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-01 16:33:59</t>
+          <t>2024-08-02 00:47:15</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>96.66176761427009</v>
+        <v>91.8246580522965</v>
       </c>
       <c r="C4" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-01 16:34:01</t>
+          <t>2024-08-02 00:47:17</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>94.84745991714172</v>
+        <v>90.73187419626102</v>
       </c>
       <c r="C5" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-01 16:34:03</t>
+          <t>2024-08-02 00:47:19</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>95.07497055502286</v>
+        <v>91.4233199347801</v>
       </c>
       <c r="C6" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-01 16:34:05</t>
+          <t>2024-08-02 00:47:21</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>93.08670366010504</v>
+        <v>89.1740850356062</v>
       </c>
       <c r="C7" t="n">
         <v>39</v>
@@ -532,66 +532,794 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-08-01 16:34:07</t>
+          <t>2024-08-02 00:47:23</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>86.86010477373431</v>
+        <v>91.86615402796529</v>
       </c>
       <c r="C8" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-08-01 16:34:09</t>
+          <t>2024-08-02 00:47:25</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>90.40116815422495</v>
+        <v>90.57818696328211</v>
       </c>
       <c r="C9" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-08-01 16:34:11</t>
+          <t>2024-08-02 00:47:27</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>92.24809728471725</v>
+        <v>91.91144387884667</v>
       </c>
       <c r="C10" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-08-01 16:34:13</t>
+          <t>2024-08-02 00:47:29</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>90.54666206727732</v>
+        <v>92.67409752090761</v>
       </c>
       <c r="C11" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-08-01 16:34:15</t>
+          <t>2024-08-02 00:47:31</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>81.20910877193739</v>
+        <v>90.52509800139639</v>
       </c>
       <c r="C12" t="n">
-        <v>43</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:47:33</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>88.43071956534283</v>
+      </c>
+      <c r="C13" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:47:35</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>85.46499954423167</v>
+      </c>
+      <c r="C14" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:47:37</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>82.68151613322509</v>
+      </c>
+      <c r="C15" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:47:39</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>84.1678755160758</v>
+      </c>
+      <c r="C16" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:47:41</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>84.39952932376684</v>
+      </c>
+      <c r="C17" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:47:43</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>84.06754753593626</v>
+      </c>
+      <c r="C18" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:47:45</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>85.28711040426694</v>
+      </c>
+      <c r="C19" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:47:48</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>88.02674388595251</v>
+      </c>
+      <c r="C20" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:47:50</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>88.44756391610284</v>
+      </c>
+      <c r="C21" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:47:52</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>88.60499379570635</v>
+      </c>
+      <c r="C22" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:47:54</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>88.50724463701005</v>
+      </c>
+      <c r="C23" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:47:56</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>87.25261329486931</v>
+      </c>
+      <c r="C24" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:47:58</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>86.27045183325347</v>
+      </c>
+      <c r="C25" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:00</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>85.43325036834969</v>
+      </c>
+      <c r="C26" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:02</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>82.99218897340862</v>
+      </c>
+      <c r="C27" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:04</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>88.10337282006583</v>
+      </c>
+      <c r="C28" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:06</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>91.60478521089517</v>
+      </c>
+      <c r="C29" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:08</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>92.14894843291826</v>
+      </c>
+      <c r="C30" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:10</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>90.23525811264346</v>
+      </c>
+      <c r="C31" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:12</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>87.7705619043945</v>
+      </c>
+      <c r="C32" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:14</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>90.72912625622278</v>
+      </c>
+      <c r="C33" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:16</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>88.66907506631679</v>
+      </c>
+      <c r="C34" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:18</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>87.62180046842363</v>
+      </c>
+      <c r="C35" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:20</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>86.22148565828756</v>
+      </c>
+      <c r="C36" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:22</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>86.50635557708799</v>
+      </c>
+      <c r="C37" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:24</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>83.97483259001602</v>
+      </c>
+      <c r="C38" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:26</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>79.03247079669843</v>
+      </c>
+      <c r="C39" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:28</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>74.69725047692287</v>
+      </c>
+      <c r="C40" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:30</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>71.80288788743411</v>
+      </c>
+      <c r="C41" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:32</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>70.05156017654866</v>
+      </c>
+      <c r="C42" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:34</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>64.12467396708071</v>
+      </c>
+      <c r="C43" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:36</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>55.6389502991379</v>
+      </c>
+      <c r="C44" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:38</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>49.352300953892</v>
+      </c>
+      <c r="C45" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:40</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>52.08382310108383</v>
+      </c>
+      <c r="C46" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:42</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>53.26759103366003</v>
+      </c>
+      <c r="C47" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:44</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>54.51591310573961</v>
+      </c>
+      <c r="C48" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:46</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>50.9663229371997</v>
+      </c>
+      <c r="C49" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:48</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>51.0885746002933</v>
+      </c>
+      <c r="C50" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:50</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>51.10532730334204</v>
+      </c>
+      <c r="C51" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:52</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>52.20837676955527</v>
+      </c>
+      <c r="C52" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:54</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>47.85256474400987</v>
+      </c>
+      <c r="C53" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:56</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>49.11196376839223</v>
+      </c>
+      <c r="C54" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:58</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>48.36386631367375</v>
+      </c>
+      <c r="C55" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:00</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>48.60546434190213</v>
+      </c>
+      <c r="C56" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:02</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>46.3659639358339</v>
+      </c>
+      <c r="C57" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:04</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>45.69489859435212</v>
+      </c>
+      <c r="C58" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:06</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>48.47401344296868</v>
+      </c>
+      <c r="C59" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:08</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>49.42294376135744</v>
+      </c>
+      <c r="C60" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:10</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>48.87702211512433</v>
+      </c>
+      <c r="C61" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:12</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>43.71989273086784</v>
+      </c>
+      <c r="C62" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:14</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>38.01338800249426</v>
+      </c>
+      <c r="C63" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:16</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>36.75868986808449</v>
+      </c>
+      <c r="C64" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:18</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>32.86028163634527</v>
+      </c>
+      <c r="C65" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:20</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>28.18495619518541</v>
+      </c>
+      <c r="C66" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:22</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>27.19917531167121</v>
+      </c>
+      <c r="C67" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:24</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>25.86201512519438</v>
+      </c>
+      <c r="C68" t="n">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -605,7 +1333,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -633,34 +1361,255 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-01 16:34:14</t>
+          <t>2024-08-02 00:48:26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Car and Truck</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>46.55 and 90.87</t>
+          <t>7.61 and 51.27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-01 16:34:15</t>
+          <t>2024-08-02 00:48:29</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.00 and 56.53</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:30</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>45.22 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:31</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>88.18 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:34</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>Truck and Car</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.00 and 23.57</t>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>9.40 and 60.68</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:48:34</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.00 and 34.87</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:11</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.00 and 74.08</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:12</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>12.04 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:14</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.00 and 43.30</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:15</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>6.85 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:17</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.00 and 19.63</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:18</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>4.04 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:19</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>44.70 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:20</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>23.10 and 0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:49:21</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>53.63 and 0.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
lane switch based on speed-difference in percentages, more tasks in todo list
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-02 20:13:08</t>
+          <t>2024-08-04 15:11:37</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>104.4392767755361</v>
+        <v>87.94661134592997</v>
       </c>
       <c r="C2" t="n">
         <v>8</v>
@@ -467,40 +467,92 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-02 20:13:10</t>
+          <t>2024-08-04 15:11:39</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>97.77957333622729</v>
+        <v>88.85274932208935</v>
       </c>
       <c r="C3" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-02 20:13:12</t>
+          <t>2024-08-04 15:11:41</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>97.51984336356436</v>
+        <v>88.54182603881817</v>
       </c>
       <c r="C4" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-02 20:13:14</t>
+          <t>2024-08-04 15:11:43</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>94.44536158396619</v>
+        <v>83.86694299403953</v>
       </c>
       <c r="C5" t="n">
-        <v>30</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-08-04 15:11:45</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>83.38592155699389</v>
+      </c>
+      <c r="C6" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-04 15:11:47</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>82.8458131050317</v>
+      </c>
+      <c r="C7" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-08-04 15:11:49</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>82.08250678513062</v>
+      </c>
+      <c r="C8" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-08-04 15:11:51</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>82.61158489264176</v>
+      </c>
+      <c r="C9" t="n">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
emergency break and start of politeness and awareness distribution
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-04 15:11:37</t>
+          <t>2024-08-04 19:40:32</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>87.94661134592997</v>
+        <v>100.1450667798633</v>
       </c>
       <c r="C2" t="n">
         <v>8</v>
@@ -467,92 +467,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-04 15:11:39</t>
+          <t>2024-08-04 19:40:34</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>88.85274932208935</v>
+        <v>92.26291639793077</v>
       </c>
       <c r="C3" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-08-04 15:11:41</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>88.54182603881817</v>
-      </c>
-      <c r="C4" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-08-04 15:11:43</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>83.86694299403953</v>
-      </c>
-      <c r="C5" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2024-08-04 15:11:45</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>83.38592155699389</v>
-      </c>
-      <c r="C6" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2024-08-04 15:11:47</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>82.8458131050317</v>
-      </c>
-      <c r="C7" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2024-08-04 15:11:49</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>82.08250678513062</v>
-      </c>
-      <c r="C8" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2024-08-04 15:11:51</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>82.61158489264176</v>
-      </c>
-      <c r="C9" t="n">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
methods and variable name changes
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,27 +454,833 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-04 19:40:32</t>
+          <t>2024-08-05 20:40:12</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100.1450667798633</v>
+        <v>84.4457612333409</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-04 19:40:34</t>
+          <t>2024-08-05 20:40:14</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>92.26291639793077</v>
+        <v>83.831215778233</v>
       </c>
       <c r="C3" t="n">
-        <v>16</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:16</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>79.20679045081511</v>
+      </c>
+      <c r="C4" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:18</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>79.07541659747979</v>
+      </c>
+      <c r="C5" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:20</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>76.84398268217089</v>
+      </c>
+      <c r="C6" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:22</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>75.74182857409946</v>
+      </c>
+      <c r="C7" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:24</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>74.41159952295018</v>
+      </c>
+      <c r="C8" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:26</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>73.59557103092239</v>
+      </c>
+      <c r="C9" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:28</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>73.8673829412616</v>
+      </c>
+      <c r="C10" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:30</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>71.3184099164794</v>
+      </c>
+      <c r="C11" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:32</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>69.50291091493385</v>
+      </c>
+      <c r="C12" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:34</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>66.73585266079488</v>
+      </c>
+      <c r="C13" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:36</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>64.28072342517761</v>
+      </c>
+      <c r="C14" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:38</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>63.91890260189304</v>
+      </c>
+      <c r="C15" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:40</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>61.51185340685008</v>
+      </c>
+      <c r="C16" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:42</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>62.99551204401815</v>
+      </c>
+      <c r="C17" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:44</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>61.21219498096455</v>
+      </c>
+      <c r="C18" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:46</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>56.71674411197418</v>
+      </c>
+      <c r="C19" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:48</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>57.31498103384463</v>
+      </c>
+      <c r="C20" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:50</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>61.14212699230703</v>
+      </c>
+      <c r="C21" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:52</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>62.76734204100413</v>
+      </c>
+      <c r="C22" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:54</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>68.71796653817962</v>
+      </c>
+      <c r="C23" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:56</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>68.5708982685167</v>
+      </c>
+      <c r="C24" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:40:58</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>68.45154058292358</v>
+      </c>
+      <c r="C25" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:00</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>68.11829508778493</v>
+      </c>
+      <c r="C26" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:03</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>72.87942724651931</v>
+      </c>
+      <c r="C27" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:05</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>72.42498980299388</v>
+      </c>
+      <c r="C28" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:07</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>74.38972484921277</v>
+      </c>
+      <c r="C29" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:09</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>72.78911065451813</v>
+      </c>
+      <c r="C30" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:11</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>72.93232400599059</v>
+      </c>
+      <c r="C31" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:13</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>70.85267930882168</v>
+      </c>
+      <c r="C32" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:15</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>72.4225320148701</v>
+      </c>
+      <c r="C33" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:17</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>72.16147088957747</v>
+      </c>
+      <c r="C34" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:19</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>70.85467012681002</v>
+      </c>
+      <c r="C35" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:21</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>71.20484234841631</v>
+      </c>
+      <c r="C36" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:23</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>72.22025312816885</v>
+      </c>
+      <c r="C37" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:25</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>71.71310908256264</v>
+      </c>
+      <c r="C38" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:27</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>64.60136691218128</v>
+      </c>
+      <c r="C39" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:29</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>65.81804658371358</v>
+      </c>
+      <c r="C40" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:31</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>64.30694378282837</v>
+      </c>
+      <c r="C41" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:33</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>60.10026590810735</v>
+      </c>
+      <c r="C42" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:35</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>54.43424624097742</v>
+      </c>
+      <c r="C43" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:37</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>51.73351675162175</v>
+      </c>
+      <c r="C44" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:39</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>49.22161229624881</v>
+      </c>
+      <c r="C45" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:41</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>43.84011820146783</v>
+      </c>
+      <c r="C46" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:43</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>40.08591845208219</v>
+      </c>
+      <c r="C47" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:45</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>40.09971442903586</v>
+      </c>
+      <c r="C48" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:47</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>40.54911156053961</v>
+      </c>
+      <c r="C49" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:49</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>41.11184930454412</v>
+      </c>
+      <c r="C50" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:51</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>46.8890959180202</v>
+      </c>
+      <c r="C51" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:53</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>49.06042700476475</v>
+      </c>
+      <c r="C52" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:55</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>50.53747967863138</v>
+      </c>
+      <c r="C53" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:57</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>50.73521347016477</v>
+      </c>
+      <c r="C54" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:59</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>51.59403377673182</v>
+      </c>
+      <c r="C55" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:42:01</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>51.64636441469018</v>
+      </c>
+      <c r="C56" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:42:03</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>51.03448821731953</v>
+      </c>
+      <c r="C57" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:42:05</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>47.84593913580318</v>
+      </c>
+      <c r="C58" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:42:07</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>48.57100719777547</v>
+      </c>
+      <c r="C59" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:42:09</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>47.67985207410288</v>
+      </c>
+      <c r="C60" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:42:11</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>45.0731586551935</v>
+      </c>
+      <c r="C61" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:42:13</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>44.37212189960569</v>
+      </c>
+      <c r="C62" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:42:15</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>45.09479509213347</v>
+      </c>
+      <c r="C63" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:42:17</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>47.84708985563245</v>
+      </c>
+      <c r="C64" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:42:19</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>48.31498104016815</v>
+      </c>
+      <c r="C65" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -488,7 +1294,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,6 +1319,40 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:31</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>3.20 and 49.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-08-05 20:41:32</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>59.88 and 0.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
unfinished version of new road
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-04 19:40:32</t>
+          <t>2024-08-20 14:43:57</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100.1450667798633</v>
+        <v>86.42145203224733</v>
       </c>
       <c r="C2" t="n">
         <v>8</v>
@@ -467,14 +467,1574 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-04 19:40:34</t>
+          <t>2024-08-20 14:43:59</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>92.26291639793077</v>
+        <v>82.51207177948444</v>
       </c>
       <c r="C3" t="n">
-        <v>16</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:01</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>79.82731552618985</v>
+      </c>
+      <c r="C4" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:03</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>79.24143210331292</v>
+      </c>
+      <c r="C5" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:05</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>76.59670198987293</v>
+      </c>
+      <c r="C6" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:07</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>76.88412451777238</v>
+      </c>
+      <c r="C7" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:09</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>74.85515373499338</v>
+      </c>
+      <c r="C8" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:11</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>72.81754900379813</v>
+      </c>
+      <c r="C9" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:13</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>71.70774498202208</v>
+      </c>
+      <c r="C10" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:15</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>71.80518712419953</v>
+      </c>
+      <c r="C11" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:17</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>69.12851540171073</v>
+      </c>
+      <c r="C12" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:19</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>71.41243995005148</v>
+      </c>
+      <c r="C13" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:21</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>68.60166790510968</v>
+      </c>
+      <c r="C14" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:23</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>69.0499734741833</v>
+      </c>
+      <c r="C15" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:25</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>70.42495923434937</v>
+      </c>
+      <c r="C16" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:27</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>71.45565498485799</v>
+      </c>
+      <c r="C17" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:29</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>70.28240765386781</v>
+      </c>
+      <c r="C18" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:31</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>69.31235561856744</v>
+      </c>
+      <c r="C19" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:33</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>68.29601371020412</v>
+      </c>
+      <c r="C20" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:35</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>67.86469996387071</v>
+      </c>
+      <c r="C21" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:37</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>68.12619499045499</v>
+      </c>
+      <c r="C22" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:39</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>68.55946232437942</v>
+      </c>
+      <c r="C23" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:41</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>68.53452693655757</v>
+      </c>
+      <c r="C24" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:43</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>68.48599041340093</v>
+      </c>
+      <c r="C25" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:45</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>67.80673488223906</v>
+      </c>
+      <c r="C26" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:47</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>68.69640758714476</v>
+      </c>
+      <c r="C27" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:49</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>72.50533370797322</v>
+      </c>
+      <c r="C28" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:51</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>74.87874213242902</v>
+      </c>
+      <c r="C29" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:53</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>74.98792936478637</v>
+      </c>
+      <c r="C30" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:55</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>74.4082495874928</v>
+      </c>
+      <c r="C31" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:57</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>74.1375325261351</v>
+      </c>
+      <c r="C32" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:44:59</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>74.78779208264271</v>
+      </c>
+      <c r="C33" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:01</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>75.67887472986364</v>
+      </c>
+      <c r="C34" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:03</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>73.72789039896172</v>
+      </c>
+      <c r="C35" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:05</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>72.34218548192548</v>
+      </c>
+      <c r="C36" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:07</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>73.38111055388414</v>
+      </c>
+      <c r="C37" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:09</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>74.02303032728132</v>
+      </c>
+      <c r="C38" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:11</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>71.47856129201986</v>
+      </c>
+      <c r="C39" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:13</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>71.4340487788094</v>
+      </c>
+      <c r="C40" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:15</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>70.74459908197426</v>
+      </c>
+      <c r="C41" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:17</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>72.86832347718855</v>
+      </c>
+      <c r="C42" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:19</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>72.77022913104835</v>
+      </c>
+      <c r="C43" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:21</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>76.05583536420002</v>
+      </c>
+      <c r="C44" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:23</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>76.45836479747931</v>
+      </c>
+      <c r="C45" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:25</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>75.80176146493616</v>
+      </c>
+      <c r="C46" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:27</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>74.01733392700383</v>
+      </c>
+      <c r="C47" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:29</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>76.69820220048794</v>
+      </c>
+      <c r="C48" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:36</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>75.29713796422001</v>
+      </c>
+      <c r="C49" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:39</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>75.61378395272746</v>
+      </c>
+      <c r="C50" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:41</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>74.78509555288097</v>
+      </c>
+      <c r="C51" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:43</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>74.54295484386232</v>
+      </c>
+      <c r="C52" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:45</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>72.37306935984697</v>
+      </c>
+      <c r="C53" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:47</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>71.88890173034281</v>
+      </c>
+      <c r="C54" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:49</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>72.76465333296413</v>
+      </c>
+      <c r="C55" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:51</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>72.54241168892447</v>
+      </c>
+      <c r="C56" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:53</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>72.73860855488684</v>
+      </c>
+      <c r="C57" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:55</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>75.37395810578393</v>
+      </c>
+      <c r="C58" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:57</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>76.35011662357057</v>
+      </c>
+      <c r="C59" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:45:59</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>76.71568265353393</v>
+      </c>
+      <c r="C60" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:01</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>77.16625365277149</v>
+      </c>
+      <c r="C61" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:03</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>78.32145839427562</v>
+      </c>
+      <c r="C62" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:05</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>78.75766438389802</v>
+      </c>
+      <c r="C63" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:07</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>79.25739663159894</v>
+      </c>
+      <c r="C64" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:09</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>80.54503039883403</v>
+      </c>
+      <c r="C65" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:11</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>79.01422134379169</v>
+      </c>
+      <c r="C66" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:13</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>76.46667743624965</v>
+      </c>
+      <c r="C67" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:15</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>78.23327554163505</v>
+      </c>
+      <c r="C68" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:17</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>76.7930757168576</v>
+      </c>
+      <c r="C69" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:19</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>75.58971220013788</v>
+      </c>
+      <c r="C70" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:21</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>72.92789236392332</v>
+      </c>
+      <c r="C71" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:24</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>72.40300806405806</v>
+      </c>
+      <c r="C72" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:26</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>72.18866502621088</v>
+      </c>
+      <c r="C73" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:28</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>73.78873101039078</v>
+      </c>
+      <c r="C74" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:30</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>72.71520835154379</v>
+      </c>
+      <c r="C75" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:32</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>75.62539760280455</v>
+      </c>
+      <c r="C76" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:34</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>76.94404275743724</v>
+      </c>
+      <c r="C77" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:36</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>75.88427752082916</v>
+      </c>
+      <c r="C78" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:38</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>75.31360546801463</v>
+      </c>
+      <c r="C79" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:40</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>75.3430449173464</v>
+      </c>
+      <c r="C80" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:42</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>78.45994631309287</v>
+      </c>
+      <c r="C81" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:44</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>76.72193415156916</v>
+      </c>
+      <c r="C82" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:46</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>76.92626270865395</v>
+      </c>
+      <c r="C83" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:48</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>78.79881772022482</v>
+      </c>
+      <c r="C84" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:50</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>77.77534838320003</v>
+      </c>
+      <c r="C85" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:52</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>72.36770053119602</v>
+      </c>
+      <c r="C86" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:54</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>74.43858584233497</v>
+      </c>
+      <c r="C87" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:56</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>74.31097915900465</v>
+      </c>
+      <c r="C88" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:46:58</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>69.94563642270921</v>
+      </c>
+      <c r="C89" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:00</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>69.28260285036302</v>
+      </c>
+      <c r="C90" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:02</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>74.36560008627369</v>
+      </c>
+      <c r="C91" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:04</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>70.25388323387683</v>
+      </c>
+      <c r="C92" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:06</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>66.3830421017022</v>
+      </c>
+      <c r="C93" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:08</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>68.71657623180248</v>
+      </c>
+      <c r="C94" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:10</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>68.93068691699405</v>
+      </c>
+      <c r="C95" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:12</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>69.49024868551791</v>
+      </c>
+      <c r="C96" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:14</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>68.22582589498259</v>
+      </c>
+      <c r="C97" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:16</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>67.57146030942911</v>
+      </c>
+      <c r="C98" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:18</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>70.0907337670377</v>
+      </c>
+      <c r="C99" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:20</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>68.47554800313287</v>
+      </c>
+      <c r="C100" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:22</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>68.37661610115988</v>
+      </c>
+      <c r="C101" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:24</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>69.76227920800312</v>
+      </c>
+      <c r="C102" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:26</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>71.4638554291006</v>
+      </c>
+      <c r="C103" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:28</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>71.28620675038252</v>
+      </c>
+      <c r="C104" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:30</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>72.92643467913952</v>
+      </c>
+      <c r="C105" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:51</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>72.8064342259901</v>
+      </c>
+      <c r="C106" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:54</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>73.70815163372463</v>
+      </c>
+      <c r="C107" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:56</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>73.50856321458458</v>
+      </c>
+      <c r="C108" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:47:58</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>79.24775579373234</v>
+      </c>
+      <c r="C109" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:48:00</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>73.83904371097209</v>
+      </c>
+      <c r="C110" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:48:02</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>76.98052111489692</v>
+      </c>
+      <c r="C111" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:48:04</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>73.38082047813906</v>
+      </c>
+      <c r="C112" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:48:06</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>75.02907319449046</v>
+      </c>
+      <c r="C113" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:48:08</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>77.02210533258108</v>
+      </c>
+      <c r="C114" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:48:10</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>77.19100108792873</v>
+      </c>
+      <c r="C115" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:48:12</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>76.90622832812637</v>
+      </c>
+      <c r="C116" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:48:14</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>75.05742537510984</v>
+      </c>
+      <c r="C117" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:48:16</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>73.05572955286291</v>
+      </c>
+      <c r="C118" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:48:18</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>72.59537260807529</v>
+      </c>
+      <c r="C119" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:48:20</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>72.7590556525556</v>
+      </c>
+      <c r="C120" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:48:22</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>73.59689633280509</v>
+      </c>
+      <c r="C121" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:48:24</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>72.2369200650737</v>
+      </c>
+      <c r="C122" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2024-08-20 14:48:26</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>73.8471523944427</v>
+      </c>
+      <c r="C123" t="n">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed field of views, added stuff to json
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:12</t>
+          <t>2024-08-20 20:07:13</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>90.87115518987385</v>
+        <v>46.07007702319964</v>
       </c>
       <c r="C2" t="n">
         <v>6</v>
@@ -467,11 +467,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:17</t>
+          <t>2024-08-20 20:07:15</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>86.22610725756415</v>
+        <v>46.68571626905674</v>
       </c>
       <c r="C3" t="n">
         <v>12</v>
@@ -480,118 +480,339 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:19</t>
+          <t>2024-08-20 20:07:17</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>90.86260134219482</v>
+        <v>46.73614301487171</v>
       </c>
       <c r="C4" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:21</t>
+          <t>2024-08-20 20:07:19</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>78.53733746169807</v>
+        <v>45.00654778894491</v>
       </c>
       <c r="C5" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:23</t>
+          <t>2024-08-20 20:07:21</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>68.20676299854883</v>
+        <v>44.47283854593196</v>
       </c>
       <c r="C6" t="n">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:25</t>
+          <t>2024-08-20 20:07:23</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>53.13304302632582</v>
+        <v>44.25753010324755</v>
       </c>
       <c r="C7" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:27</t>
+          <t>2024-08-20 20:07:25</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>46.25051504842485</v>
+        <v>42.08148493204431</v>
       </c>
       <c r="C8" t="n">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:29</t>
+          <t>2024-08-20 20:07:27</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>32.28639826130397</v>
+        <v>40.12209562656724</v>
       </c>
       <c r="C9" t="n">
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:31</t>
+          <t>2024-08-20 20:07:29</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>24.38369684343937</v>
+        <v>38.62306089772105</v>
       </c>
       <c r="C10" t="n">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:33</t>
+          <t>2024-08-20 20:07:31</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>21.60910384184912</v>
+        <v>34.6755661717304</v>
       </c>
       <c r="C11" t="n">
-        <v>60</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:35</t>
+          <t>2024-08-20 20:07:33</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>17.33756226266445</v>
+        <v>30.47304625739552</v>
       </c>
       <c r="C12" t="n">
-        <v>63</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:07:35</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>25.7111187852357</v>
+      </c>
+      <c r="C13" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:07:37</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>19.88076169218955</v>
+      </c>
+      <c r="C14" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:07:39</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>19.7883157606013</v>
+      </c>
+      <c r="C15" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:07:41</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>16.54083733766959</v>
+      </c>
+      <c r="C16" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:07:43</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>14.61677850968699</v>
+      </c>
+      <c r="C17" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:07:45</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>14.08305693466309</v>
+      </c>
+      <c r="C18" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:07:47</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>13.24840950078344</v>
+      </c>
+      <c r="C19" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:07:49</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>9.474456357197411</v>
+      </c>
+      <c r="C20" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:07:51</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>8.388228323535746</v>
+      </c>
+      <c r="C21" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:07:53</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>8.096077864805677</v>
+      </c>
+      <c r="C22" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:07:55</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>7.316246588503244</v>
+      </c>
+      <c r="C23" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:07:57</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>8.096662506099912</v>
+      </c>
+      <c r="C24" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:07:59</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>8.155587986840546</v>
+      </c>
+      <c r="C25" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:08:01</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>6.27096484442682</v>
+      </c>
+      <c r="C26" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:08:03</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>6.164327355047057</v>
+      </c>
+      <c r="C27" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:08:05</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>5.569760559848789</v>
+      </c>
+      <c r="C28" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-08-20 20:08:07</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>4.541220809264694</v>
+      </c>
+      <c r="C29" t="n">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -605,7 +826,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -633,323 +854,85 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:20</t>
+          <t>2024-08-20 20:07:29</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Truck and Truck</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>75.89 and 95.71</t>
+          <t>6.77 and 17.90</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:20</t>
+          <t>2024-08-20 20:07:32</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>97.96 and 0.00</t>
+          <t>29.48 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:21</t>
+          <t>2024-08-20 20:07:33</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Truck and Car</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>93.72 and 0.00</t>
+          <t>30.26 and 0.00</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:22</t>
+          <t>2024-08-20 20:07:36</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>76.49 and 0.00</t>
+          <t>0.00 and 35.72</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-20 15:01:22</t>
+          <t>2024-08-20 20:07:37</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>90.73 and 88.44</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2024-08-20 15:01:22</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>74.88 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2024-08-20 15:01:23</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>88.39 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2024-08-20 15:01:23</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>85.36 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2024-08-20 15:01:24</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Truck and Car</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>78.32 and 105.61</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2024-08-20 15:01:24</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Truck and Car</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>86.28 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2024-08-20 15:01:24</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>110.18 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2024-08-20 15:01:24</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Car and Truck</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>77.78 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2024-08-20 15:01:26</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>78.40 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2024-08-20 15:01:27</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>75.70 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2024-08-20 15:01:27</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>100.35 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2024-08-20 15:01:28</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>98.08 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2024-08-20 15:01:29</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>90.95 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2024-08-20 15:01:30</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>93.59 and 0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2024-08-20 15:01:30</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>71.95 and 0.00</t>
+          <t>45.17 and 0.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changing of json unfinished
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,24 +454,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:35</t>
+          <t>2024-08-21 17:43:46</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>56.20259132760435</v>
+        <v>53.2597868721498</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:37</t>
+          <t>2024-08-21 17:43:48</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>55.91799014703505</v>
+        <v>53.3096261348934</v>
       </c>
       <c r="C3" t="n">
         <v>13</v>
@@ -480,50 +480,50 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:39</t>
+          <t>2024-08-21 17:43:50</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>54.74386856781135</v>
+        <v>52.88633371650054</v>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:41</t>
+          <t>2024-08-21 17:43:52</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>53.33349220763156</v>
+        <v>50.84237885885849</v>
       </c>
       <c r="C5" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:43</t>
+          <t>2024-08-21 17:43:55</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>52.87857320122561</v>
+        <v>45.85710907513953</v>
       </c>
       <c r="C6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:45</t>
+          <t>2024-08-21 17:43:57</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46.05820854228062</v>
+        <v>39.65579930384778</v>
       </c>
       <c r="C7" t="n">
         <v>27</v>
@@ -532,11 +532,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:47</t>
+          <t>2024-08-21 17:43:59</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>35.7315644382626</v>
+        <v>40.37960121286115</v>
       </c>
       <c r="C8" t="n">
         <v>28</v>
@@ -545,11 +545,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:49</t>
+          <t>2024-08-21 17:44:01</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>37.53809477153479</v>
+        <v>38.29742760463628</v>
       </c>
       <c r="C9" t="n">
         <v>27</v>
@@ -558,89 +558,89 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:51</t>
+          <t>2024-08-21 17:44:03</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>32.24250722205096</v>
+        <v>36.75830900142348</v>
       </c>
       <c r="C10" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:53</t>
+          <t>2024-08-21 17:44:05</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>35.98561417714961</v>
+        <v>39.2270736932723</v>
       </c>
       <c r="C11" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:55</t>
+          <t>2024-08-21 17:44:07</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>31.20516287095538</v>
+        <v>34.96951146285748</v>
       </c>
       <c r="C12" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:57</t>
+          <t>2024-08-21 17:44:09</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>29.95844526063537</v>
+        <v>31.93928113526318</v>
       </c>
       <c r="C13" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:59</t>
+          <t>2024-08-21 17:44:11</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>30.42405247786244</v>
+        <v>30.87915370635895</v>
       </c>
       <c r="C14" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:01</t>
+          <t>2024-08-21 17:44:13</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>30.68706566352703</v>
+        <v>30.86046802726679</v>
       </c>
       <c r="C15" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:03</t>
+          <t>2024-08-21 17:44:15</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>33.93307759558655</v>
+        <v>34.8145223948564</v>
       </c>
       <c r="C16" t="n">
         <v>31</v>
@@ -649,92 +649,547 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:05</t>
+          <t>2024-08-21 17:44:17</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>27.29977551958575</v>
+        <v>32.47670200564293</v>
       </c>
       <c r="C17" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:07</t>
+          <t>2024-08-21 17:44:19</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>33.5094895948509</v>
+        <v>33.66226437536362</v>
       </c>
       <c r="C18" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:09</t>
+          <t>2024-08-21 17:44:21</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>28.31356670610524</v>
+        <v>33.09571951800906</v>
       </c>
       <c r="C19" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:11</t>
+          <t>2024-08-21 17:44:23</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>33.18471326250101</v>
+        <v>38.59116503744637</v>
       </c>
       <c r="C20" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:13</t>
+          <t>2024-08-21 17:44:25</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>27.0640692761312</v>
+        <v>34.69362189409538</v>
       </c>
       <c r="C21" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:15</t>
+          <t>2024-08-21 17:44:27</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>26.6226933985967</v>
+        <v>34.10056881538849</v>
       </c>
       <c r="C22" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:17</t>
+          <t>2024-08-21 17:44:29</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>29.62716079111139</v>
+        <v>33.66405266894405</v>
       </c>
       <c r="C23" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:31</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>26.17422947859876</v>
+      </c>
+      <c r="C24" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:33</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>32.31625505677929</v>
+      </c>
+      <c r="C25" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:35</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>27.34599918758866</v>
+      </c>
+      <c r="C26" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:37</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>25.20376652458257</v>
+      </c>
+      <c r="C27" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:39</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>34.65633244540913</v>
+      </c>
+      <c r="C28" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:41</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>32.02488864699885</v>
+      </c>
+      <c r="C29" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:43</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>31.7561179230039</v>
+      </c>
+      <c r="C30" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:45</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>34.44263519006502</v>
+      </c>
+      <c r="C31" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:47</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>28.91155524530594</v>
+      </c>
+      <c r="C32" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:49</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>31.2247647270954</v>
+      </c>
+      <c r="C33" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:51</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>33.31848549298379</v>
+      </c>
+      <c r="C34" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:53</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>33.28308946787771</v>
+      </c>
+      <c r="C35" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:55</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>31.51743266704381</v>
+      </c>
+      <c r="C36" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:57</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>27.54575450675285</v>
+      </c>
+      <c r="C37" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:59</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>29.62615157164711</v>
+      </c>
+      <c r="C38" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:01</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>32.13586844328807</v>
+      </c>
+      <c r="C39" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:03</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>31.95387765513365</v>
+      </c>
+      <c r="C40" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:05</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>34.9106350205066</v>
+      </c>
+      <c r="C41" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:07</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>30.52806368336728</v>
+      </c>
+      <c r="C42" t="n">
         <v>34</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:09</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>25.09747607378401</v>
+      </c>
+      <c r="C43" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:11</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>25.77450295835182</v>
+      </c>
+      <c r="C44" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:13</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>27.00591701907633</v>
+      </c>
+      <c r="C45" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:15</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>28.41774230506413</v>
+      </c>
+      <c r="C46" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:17</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>27.2860076742514</v>
+      </c>
+      <c r="C47" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:19</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>29.31387494205724</v>
+      </c>
+      <c r="C48" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:21</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>26.64486446228091</v>
+      </c>
+      <c r="C49" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:23</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>26.73714009450719</v>
+      </c>
+      <c r="C50" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:25</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>24.564870681794</v>
+      </c>
+      <c r="C51" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:27</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>25.10075636602006</v>
+      </c>
+      <c r="C52" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:29</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>22.29508633083137</v>
+      </c>
+      <c r="C53" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:31</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>19.38186955297007</v>
+      </c>
+      <c r="C54" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:33</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>17.6735899755845</v>
+      </c>
+      <c r="C55" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:35</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>18.46172362378111</v>
+      </c>
+      <c r="C56" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:37</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>16.83440958380139</v>
+      </c>
+      <c r="C57" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:40</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>15.72603118014481</v>
+      </c>
+      <c r="C58" t="n">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -748,7 +1203,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -781,7 +1236,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:44</t>
+          <t>2024-08-21 17:43:54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -791,7 +1246,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>46.37 and 46.28</t>
+          <t>45.36 and 56.25</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -801,17 +1256,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:46</t>
+          <t>2024-08-21 17:43:57</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Truck and Car</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.00 and 60.11</t>
+          <t>0.00 and 52.72</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -821,7 +1276,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:48</t>
+          <t>2024-08-21 17:43:59</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -831,7 +1286,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>48.47 and 42.20</t>
+          <t>51.88 and 40.09</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -841,17 +1296,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:50</t>
+          <t>2024-08-21 17:44:01</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>58.26 and 47.47</t>
+          <t>28.73 and 47.09</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -861,7 +1316,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:53</t>
+          <t>2024-08-21 17:44:05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -871,7 +1326,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>64.32 and 47.71</t>
+          <t>42.41 and 47.40</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -881,17 +1336,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:54</t>
+          <t>2024-08-21 17:44:06</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Truck and Car</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>33.40 and 37.27</t>
+          <t>0.00 and 40.57</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -901,17 +1356,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:57</t>
+          <t>2024-08-21 17:44:09</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Truck and Car</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>35.73 and 49.03</t>
+          <t>3.03 and 48.20</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -921,7 +1376,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-08-21 15:50:59</t>
+          <t>2024-08-21 17:44:10</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -931,7 +1386,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>18.64 and 48.30</t>
+          <t>34.15 and 61.49</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -941,7 +1396,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:03</t>
+          <t>2024-08-21 17:44:14</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -951,7 +1406,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>34.25 and 49.88</t>
+          <t>57.60 and 51.34</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -961,17 +1416,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:03</t>
+          <t>2024-08-21 17:44:15</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Truck and Car</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>9.00 and 47.08</t>
+          <t>36.20 and 50.52</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -981,7 +1436,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:06</t>
+          <t>2024-08-21 17:44:18</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -991,7 +1446,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.00 and 31.67</t>
+          <t>0.00 and 23.76</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -1001,7 +1456,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:07</t>
+          <t>2024-08-21 17:44:18</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1011,7 +1466,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>46.54 and 50.66</t>
+          <t>65.22 and 40.38</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -1021,27 +1476,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:08</t>
+          <t>2024-08-21 17:44:20</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Truck and Car</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>16.99 and 51.44</t>
+          <t>32.49 and 0.00</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:11</t>
+          <t>2024-08-21 17:44:21</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1051,67 +1506,67 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>57.91 and 47.23</t>
+          <t>0.00 and 58.69</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:12</t>
+          <t>2024-08-21 17:44:23</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Car and Truck</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>5.25 and 28.53</t>
+          <t>48.41 and 37.20</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:15</t>
+          <t>2024-08-21 17:44:29</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Car and Truck</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>37.27 and 40.86</t>
+          <t>55.84 and 45.41</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:17</t>
+          <t>2024-08-21 17:44:29</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Car and Truck</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>36.39 and 0.00</t>
+          <t>0.00 and 59.09</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1121,7 +1576,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2024-08-21 15:51:18</t>
+          <t>2024-08-21 17:44:34</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1131,11 +1586,231 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>35.34 and 0.00</t>
+          <t>43.81 and 44.49</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>16</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:34</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>33.39 and 62.28</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:39</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>38.69 and 53.66</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:40</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>57.29 and 52.54</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:45</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>63.71 and 44.16</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:45</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>52.51 and 31.50</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:50</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>54.36 and 45.10</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:54</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0.00 and 46.19</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:56</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>47.22 and 46.27</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:44:59</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>55.15 and 40.70</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:01</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>56.16 and 47.61</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-08-21 17:45:07</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>38.43 and 55.51</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
quarter-working junction - turns but lots of accidents
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,53 +454,235 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-21 19:51:40</t>
+          <t>2024-08-22 18:10:47</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>52.44934683181798</v>
+        <v>50.78206774004448</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-21 19:51:42</t>
+          <t>2024-08-22 18:10:49</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>52.64854191853105</v>
+        <v>50.26977158884897</v>
       </c>
       <c r="C3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-21 19:53:17</t>
+          <t>2024-08-22 18:10:51</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>52.33903900597083</v>
+        <v>52.23679678239277</v>
       </c>
       <c r="C4" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-21 19:53:19</t>
+          <t>2024-08-22 18:10:53</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>51.5477852861154</v>
+        <v>54.26354674871339</v>
       </c>
       <c r="C5" t="n">
         <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:10:55</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>47.62661735562251</v>
+      </c>
+      <c r="C6" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:10:57</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>47.38531304538915</v>
+      </c>
+      <c r="C7" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:10:59</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>35.94129370198269</v>
+      </c>
+      <c r="C8" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:01</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>36.5052821850792</v>
+      </c>
+      <c r="C9" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:03</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>45.46172357303922</v>
+      </c>
+      <c r="C10" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:05</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>34.00479330213628</v>
+      </c>
+      <c r="C11" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:07</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>43.25765093338282</v>
+      </c>
+      <c r="C12" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:09</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>42.29515067463542</v>
+      </c>
+      <c r="C13" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:11</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>52.44730393024552</v>
+      </c>
+      <c r="C14" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:13</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>42.77169918724547</v>
+      </c>
+      <c r="C15" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:15</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>34.48240939036887</v>
+      </c>
+      <c r="C16" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:17</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>41.22569760117101</v>
+      </c>
+      <c r="C17" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:19</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>48.16745391638945</v>
+      </c>
+      <c r="C18" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:21</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>47.40192046541741</v>
+      </c>
+      <c r="C19" t="n">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -514,7 +696,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,6 +726,306 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:10:54</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>42.43 and 32.19</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:10:56</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>58.21 and 40.46</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:10:59</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.00 and 65.00</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:10:59</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.00 and 53.67</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:02</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>55.15 and 0.00</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:03</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.00 and 40.12</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:03</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>58.20 and 0.00</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:05</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>62.12 and 0.00</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:07</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>52.43 and 7.56</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:08</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>47.16 and 0.00</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:13</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.04 and 55.48</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:14</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.00 and 50.47</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:16</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0.00 and 58.61</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:18</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0.00 and 49.92</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-22 18:11:18</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>61.00 and 0.00</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
continous driving all junctions
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,27 +454,443 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-22 20:31:42</t>
+          <t>2024-08-22 23:21:29</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>54.28385778322846</v>
+        <v>50.7562999187541</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-22 20:31:44</t>
+          <t>2024-08-22 23:21:31</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>55.49353681360942</v>
+        <v>57.17583602451682</v>
       </c>
       <c r="C3" t="n">
-        <v>11</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:33</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>51.6582693434123</v>
+      </c>
+      <c r="C4" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:35</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>51.80516693022747</v>
+      </c>
+      <c r="C5" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:37</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>49.59439408910465</v>
+      </c>
+      <c r="C6" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:39</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>41.53237173275736</v>
+      </c>
+      <c r="C7" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:41</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>35.45276113372355</v>
+      </c>
+      <c r="C8" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:43</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>47.12841429152716</v>
+      </c>
+      <c r="C9" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:45</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>45.96187959783757</v>
+      </c>
+      <c r="C10" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:47</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>45.56572322390616</v>
+      </c>
+      <c r="C11" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:49</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>41.94287249991656</v>
+      </c>
+      <c r="C12" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:51</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>48.13670014890594</v>
+      </c>
+      <c r="C13" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:53</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>45.01821904559821</v>
+      </c>
+      <c r="C14" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:55</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>46.04346255493876</v>
+      </c>
+      <c r="C15" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:57</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>42.50415145498472</v>
+      </c>
+      <c r="C16" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:59</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>46.39709858162221</v>
+      </c>
+      <c r="C17" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:01</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>48.28977957717415</v>
+      </c>
+      <c r="C18" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:04</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>47.09990002587454</v>
+      </c>
+      <c r="C19" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:06</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>47.83851514129372</v>
+      </c>
+      <c r="C20" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:08</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>43.35359397925863</v>
+      </c>
+      <c r="C21" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:10</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>34.64754207108391</v>
+      </c>
+      <c r="C22" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:12</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>33.27398738466093</v>
+      </c>
+      <c r="C23" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:14</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>39.94681231630955</v>
+      </c>
+      <c r="C24" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:16</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>36.65762401360691</v>
+      </c>
+      <c r="C25" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:18</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>37.91643276685179</v>
+      </c>
+      <c r="C26" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:20</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>32.33250595860922</v>
+      </c>
+      <c r="C27" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:22</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>44.59632469890458</v>
+      </c>
+      <c r="C28" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:24</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>49.11429460491107</v>
+      </c>
+      <c r="C29" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:26</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>48.11975813911408</v>
+      </c>
+      <c r="C30" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:28</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>46.5272329214261</v>
+      </c>
+      <c r="C31" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:30</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>45.48999321564249</v>
+      </c>
+      <c r="C32" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:32</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>42.37124612647354</v>
+      </c>
+      <c r="C33" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:34</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>35.04710376292122</v>
+      </c>
+      <c r="C34" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:36</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>43.66752401891386</v>
+      </c>
+      <c r="C35" t="n">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -488,7 +904,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,6 +934,346 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:38</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.00 and 34.63</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:39</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>41.66 and 0.00</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:40</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>31.48 and 32.77</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:42</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>37.99 and 0.00</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:48</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>28.62 and 23.13</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:49</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>23.44 and 0.00</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:50</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.00 and 30.85</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:21:56</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>33.14 and 25.84</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:09</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>34.99 and 43.66</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:09</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.00 and 39.07</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:13</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.00 and 29.66</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:17</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.00 and 35.94</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:19</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>33.27 and 0.00</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:32</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0.00 and 32.30</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:33</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0.00 and 26.28</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:34</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>36.62 and 0.00</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-08-22 23:22:34</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>33.58 and 0.00</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
start of hazards handle
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-25 16:58:50</t>
+          <t>2024-08-25 21:16:20</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>48.62914731284807</v>
+        <v>42.4964350850333</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
@@ -467,53 +467,66 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-25 16:58:52</t>
+          <t>2024-08-25 21:16:22</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>51.21571936382904</v>
+        <v>42.33126581995717</v>
       </c>
       <c r="C3" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-25 16:58:54</t>
+          <t>2024-08-25 21:16:24</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>52.71772236089878</v>
+        <v>43.87835996264035</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-25 16:58:56</t>
+          <t>2024-08-25 21:16:26</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>51.21593542104949</v>
+        <v>43.00827997015465</v>
       </c>
       <c r="C5" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-25 16:58:58</t>
+          <t>2024-08-25 21:16:28</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>50.81251242420966</v>
+        <v>41.63382863258526</v>
       </c>
       <c r="C6" t="n">
         <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-25 21:16:30</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>31.75084319358936</v>
+      </c>
+      <c r="C7" t="n">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -527,7 +540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,6 +570,26 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-08-25 21:16:30</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>35.89 and 39.31</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
kind of working speed limit sign
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-25 21:16:20</t>
+          <t>2024-08-26 15:04:47</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>42.4964350850333</v>
+        <v>44.13390296570707</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
@@ -467,37 +467,37 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-25 21:16:22</t>
+          <t>2024-08-26 15:04:49</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>42.33126581995717</v>
+        <v>42.16621551850734</v>
       </c>
       <c r="C3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-25 21:16:24</t>
+          <t>2024-08-26 15:04:51</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>43.87835996264035</v>
+        <v>42.38298800889578</v>
       </c>
       <c r="C4" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-25 21:16:26</t>
+          <t>2024-08-26 15:04:53</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>43.00827997015465</v>
+        <v>44.16098196112721</v>
       </c>
       <c r="C5" t="n">
         <v>11</v>
@@ -506,27 +506,144 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-25 21:16:28</t>
+          <t>2024-08-26 15:06:01</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>41.63382863258526</v>
+        <v>42.22672922880924</v>
       </c>
       <c r="C6" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-25 21:16:30</t>
+          <t>2024-08-26 15:06:12</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>31.75084319358936</v>
+        <v>42.15700632867082</v>
       </c>
       <c r="C7" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-08-26 15:06:17</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>42.77970146747748</v>
+      </c>
+      <c r="C8" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-08-26 15:06:19</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>42.73019503803481</v>
+      </c>
+      <c r="C9" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-08-26 15:09:01</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>43.33023722596015</v>
+      </c>
+      <c r="C10" t="n">
         <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-08-26 15:09:03</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>43.39401072519414</v>
+      </c>
+      <c r="C11" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-08-26 15:09:05</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>43.31036399285087</v>
+      </c>
+      <c r="C12" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-26 15:09:40</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>43.11456799213904</v>
+      </c>
+      <c r="C13" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-08-26 15:09:42</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>42.98245919569164</v>
+      </c>
+      <c r="C14" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-26 15:09:44</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>38.53016086544418</v>
+      </c>
+      <c r="C15" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-26 15:09:46</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>42.97772545656818</v>
+      </c>
+      <c r="C16" t="n">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -540,7 +657,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -570,26 +687,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-08-25 21:16:30</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>35.89 and 39.31</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
starting of speed decison make
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-26 15:04:47</t>
+          <t>2024-08-27 14:48:53</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>44.13390296570707</v>
+        <v>33.82234123357149</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
@@ -467,24 +467,24 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-26 15:04:49</t>
+          <t>2024-08-27 14:48:55</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>42.16621551850734</v>
+        <v>34.70162069399007</v>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-26 15:04:51</t>
+          <t>2024-08-27 14:48:57</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>42.38298800889578</v>
+        <v>37.03816020955322</v>
       </c>
       <c r="C4" t="n">
         <v>9</v>
@@ -493,11 +493,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-26 15:04:53</t>
+          <t>2024-08-27 14:48:59</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>44.16098196112721</v>
+        <v>39.21010669201421</v>
       </c>
       <c r="C5" t="n">
         <v>11</v>
@@ -506,144 +506,339 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-26 15:06:01</t>
+          <t>2024-08-27 14:49:01</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>42.22672922880924</v>
+        <v>38.46490281879766</v>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-26 15:06:12</t>
+          <t>2024-08-27 14:49:03</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>42.15700632867082</v>
+        <v>39.29688538284288</v>
       </c>
       <c r="C7" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-08-26 15:06:17</t>
+          <t>2024-08-27 14:49:05</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>42.77970146747748</v>
+        <v>39.27772065768913</v>
       </c>
       <c r="C8" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-08-26 15:06:19</t>
+          <t>2024-08-27 14:49:07</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>42.73019503803481</v>
+        <v>36.67309280329896</v>
       </c>
       <c r="C9" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-08-26 15:09:01</t>
+          <t>2024-08-27 14:49:09</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>43.33023722596015</v>
+        <v>28.06036210561786</v>
       </c>
       <c r="C10" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-08-26 15:09:03</t>
+          <t>2024-08-27 14:49:11</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>43.39401072519414</v>
+        <v>33.72263203589913</v>
       </c>
       <c r="C11" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-08-26 15:09:05</t>
+          <t>2024-08-27 14:49:14</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>43.31036399285087</v>
+        <v>33.58718957253446</v>
       </c>
       <c r="C12" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2024-08-26 15:09:40</t>
+          <t>2024-08-27 14:49:16</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>43.11456799213904</v>
+        <v>28.28250633813379</v>
       </c>
       <c r="C13" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2024-08-26 15:09:42</t>
+          <t>2024-08-27 14:49:18</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>42.98245919569164</v>
+        <v>31.77988347368915</v>
       </c>
       <c r="C14" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2024-08-26 15:09:44</t>
+          <t>2024-08-27 14:49:20</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>38.53016086544418</v>
+        <v>29.75150592701652</v>
       </c>
       <c r="C15" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2024-08-26 15:09:46</t>
+          <t>2024-08-27 14:49:22</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>42.97772545656818</v>
+        <v>29.91431503230635</v>
       </c>
       <c r="C16" t="n">
-        <v>17</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:24</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>27.26311660794591</v>
+      </c>
+      <c r="C17" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:26</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>27.44778645551681</v>
+      </c>
+      <c r="C18" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:28</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>21.12725701441377</v>
+      </c>
+      <c r="C19" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:30</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>21.47993317810211</v>
+      </c>
+      <c r="C20" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:32</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>24.38316892234656</v>
+      </c>
+      <c r="C21" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:34</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>20.78166059720699</v>
+      </c>
+      <c r="C22" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:36</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>24.06209510791275</v>
+      </c>
+      <c r="C23" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:38</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>24.88620965920845</v>
+      </c>
+      <c r="C24" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:40</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>21.39336173405988</v>
+      </c>
+      <c r="C25" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:42</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>18.95274755377982</v>
+      </c>
+      <c r="C26" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:44</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>24.43699718643903</v>
+      </c>
+      <c r="C27" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:46</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>26.24975857312631</v>
+      </c>
+      <c r="C28" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:48</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>25.98849097744464</v>
+      </c>
+      <c r="C29" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:50</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>25.74623652075309</v>
+      </c>
+      <c r="C30" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:52</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>26.82238415272914</v>
+      </c>
+      <c r="C31" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -657,7 +852,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -687,6 +882,126 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:08</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>26.27 and 29.66</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:09</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>29.56 and 0.00</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:27</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>38.18 and 43.76</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:30</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.00 and 26.17</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:40</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>31.16 and 41.78</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-27 14:49:41</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>33.89 and 0.00</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor of accelerate_and_break, and of Hazard
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-27 14:48:53</t>
+          <t>2024-08-27 21:28:26</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>33.82234123357149</v>
+        <v>40.02594850353584</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
@@ -467,37 +467,37 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-27 14:48:55</t>
+          <t>2024-08-27 21:28:28</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>34.70162069399007</v>
+        <v>48.63462475601763</v>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-27 14:48:57</t>
+          <t>2024-08-27 21:28:30</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>37.03816020955322</v>
+        <v>46.34341826047311</v>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-27 14:48:59</t>
+          <t>2024-08-27 21:28:32</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>39.21010669201421</v>
+        <v>47.12549901152027</v>
       </c>
       <c r="C5" t="n">
         <v>11</v>
@@ -506,11 +506,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:01</t>
+          <t>2024-08-27 21:28:34</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>38.46490281879766</v>
+        <v>44.96126186781996</v>
       </c>
       <c r="C6" t="n">
         <v>14</v>
@@ -519,297 +519,297 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:03</t>
+          <t>2024-08-27 21:28:36</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>39.29688538284288</v>
+        <v>44.12630965542294</v>
       </c>
       <c r="C7" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:05</t>
+          <t>2024-08-27 21:28:38</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>39.27772065768913</v>
+        <v>36.83478505847535</v>
       </c>
       <c r="C8" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:07</t>
+          <t>2024-08-27 21:28:40</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>36.67309280329896</v>
+        <v>44.56468421250889</v>
       </c>
       <c r="C9" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:09</t>
+          <t>2024-08-27 21:28:42</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>28.06036210561786</v>
+        <v>41.3034741483392</v>
       </c>
       <c r="C10" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:11</t>
+          <t>2024-08-27 21:28:44</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>33.72263203589913</v>
+        <v>47.15567190705765</v>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:14</t>
+          <t>2024-08-27 21:28:46</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>33.58718957253446</v>
+        <v>38.7747139225344</v>
       </c>
       <c r="C12" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:16</t>
+          <t>2024-08-27 21:28:48</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>28.28250633813379</v>
+        <v>30.54502384136241</v>
       </c>
       <c r="C13" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:18</t>
+          <t>2024-08-27 21:28:50</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>31.77988347368915</v>
+        <v>37.89724118455234</v>
       </c>
       <c r="C14" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:20</t>
+          <t>2024-08-27 21:28:52</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>29.75150592701652</v>
+        <v>36.50009132936643</v>
       </c>
       <c r="C15" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:22</t>
+          <t>2024-08-27 21:28:54</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>29.91431503230635</v>
+        <v>24.52353658128494</v>
       </c>
       <c r="C16" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:24</t>
+          <t>2024-08-27 21:28:56</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>27.26311660794591</v>
+        <v>38.42062143576025</v>
       </c>
       <c r="C17" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:26</t>
+          <t>2024-08-27 21:28:58</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>27.44778645551681</v>
+        <v>31.18559241644166</v>
       </c>
       <c r="C18" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:28</t>
+          <t>2024-08-27 21:29:00</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>21.12725701441377</v>
+        <v>32.83124440759135</v>
       </c>
       <c r="C19" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:30</t>
+          <t>2024-08-27 21:29:02</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>21.47993317810211</v>
+        <v>44.48627924356973</v>
       </c>
       <c r="C20" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:32</t>
+          <t>2024-08-27 21:29:04</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>24.38316892234656</v>
+        <v>38.72174025699398</v>
       </c>
       <c r="C21" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:34</t>
+          <t>2024-08-27 21:29:06</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>20.78166059720699</v>
+        <v>36.60521789394152</v>
       </c>
       <c r="C22" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:36</t>
+          <t>2024-08-27 21:29:08</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>24.06209510791275</v>
+        <v>36.63824046202497</v>
       </c>
       <c r="C23" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:38</t>
+          <t>2024-08-27 21:29:10</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>24.88620965920845</v>
+        <v>46.86543941054851</v>
       </c>
       <c r="C24" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:40</t>
+          <t>2024-08-27 21:29:12</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>21.39336173405988</v>
+        <v>35.56932448895882</v>
       </c>
       <c r="C25" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:42</t>
+          <t>2024-08-27 21:29:14</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>18.95274755377982</v>
+        <v>42.51679130714032</v>
       </c>
       <c r="C26" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:44</t>
+          <t>2024-08-27 21:29:16</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>24.43699718643903</v>
+        <v>39.28789118734366</v>
       </c>
       <c r="C27" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:46</t>
+          <t>2024-08-27 21:29:18</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>26.24975857312631</v>
+        <v>38.83235780587304</v>
       </c>
       <c r="C28" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:48</t>
+          <t>2024-08-27 21:29:20</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>25.98849097744464</v>
+        <v>36.99918250031377</v>
       </c>
       <c r="C29" t="n">
         <v>21</v>
@@ -818,27 +818,1210 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:50</t>
+          <t>2024-08-27 21:29:22</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>25.74623652075309</v>
+        <v>39.97538166048453</v>
       </c>
       <c r="C30" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:52</t>
+          <t>2024-08-27 21:29:24</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>26.82238415272914</v>
+        <v>38.33283333520905</v>
       </c>
       <c r="C31" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:29:26</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>40.28467750691467</v>
+      </c>
+      <c r="C32" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:29:28</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>28.59867445907127</v>
+      </c>
+      <c r="C33" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:29:30</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>37.02892019100605</v>
+      </c>
+      <c r="C34" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:29:32</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>38.5309727742064</v>
+      </c>
+      <c r="C35" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:29:34</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>41.50233276925238</v>
+      </c>
+      <c r="C36" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:29:36</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>42.51821506571499</v>
+      </c>
+      <c r="C37" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:01</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>47.84909068541635</v>
+      </c>
+      <c r="C38" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:03</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>44.20135905954171</v>
+      </c>
+      <c r="C39" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:05</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>43.55352225574953</v>
+      </c>
+      <c r="C40" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:07</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>42.75898578220787</v>
+      </c>
+      <c r="C41" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:09</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>42.95597509263507</v>
+      </c>
+      <c r="C42" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:11</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>26.24121387457992</v>
+      </c>
+      <c r="C43" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:13</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>26.85274040754234</v>
+      </c>
+      <c r="C44" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:15</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>43.69138404585277</v>
+      </c>
+      <c r="C45" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:17</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>34.41134951297835</v>
+      </c>
+      <c r="C46" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:19</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>31.85587185732415</v>
+      </c>
+      <c r="C47" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:21</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>24.00464649886975</v>
+      </c>
+      <c r="C48" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:23</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>37.85694170330785</v>
+      </c>
+      <c r="C49" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:25</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>43.17555218565101</v>
+      </c>
+      <c r="C50" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:27</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>31.50518663425973</v>
+      </c>
+      <c r="C51" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:29</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>35.5485972576531</v>
+      </c>
+      <c r="C52" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:31</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>20.35996234188621</v>
+      </c>
+      <c r="C53" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:33</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>41.61245927517656</v>
+      </c>
+      <c r="C54" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:35</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>39.92730632273698</v>
+      </c>
+      <c r="C55" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:37</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>41.22144998329975</v>
+      </c>
+      <c r="C56" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:39</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>33.69646162224405</v>
+      </c>
+      <c r="C57" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:41</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>39.2664430980241</v>
+      </c>
+      <c r="C58" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:43</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>42.41050638087449</v>
+      </c>
+      <c r="C59" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:45</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>47.91769303295316</v>
+      </c>
+      <c r="C60" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:47</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>41.23730288313681</v>
+      </c>
+      <c r="C61" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:49</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>34.82775182916041</v>
+      </c>
+      <c r="C62" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:51</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>36.85736619646811</v>
+      </c>
+      <c r="C63" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:53</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>34.57823699083947</v>
+      </c>
+      <c r="C64" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:55</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>43.41335105247909</v>
+      </c>
+      <c r="C65" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:57</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>37.69452016172852</v>
+      </c>
+      <c r="C66" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:59</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>45.30738582634181</v>
+      </c>
+      <c r="C67" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:01</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>45.64756853436316</v>
+      </c>
+      <c r="C68" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:03</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>47.30861895041792</v>
+      </c>
+      <c r="C69" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:05</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>43.51345930053807</v>
+      </c>
+      <c r="C70" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:07</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>39.97437296566079</v>
+      </c>
+      <c r="C71" t="n">
         <v>22</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:09</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>36.97677391637695</v>
+      </c>
+      <c r="C72" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:11</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>42.72630159220384</v>
+      </c>
+      <c r="C73" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:13</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>34.58139537849686</v>
+      </c>
+      <c r="C74" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:15</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>35.49484262718137</v>
+      </c>
+      <c r="C75" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:17</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>45.10438045309695</v>
+      </c>
+      <c r="C76" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:19</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>34.67958855157436</v>
+      </c>
+      <c r="C77" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:21</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>32.14918364258885</v>
+      </c>
+      <c r="C78" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:23</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>42.7038460648326</v>
+      </c>
+      <c r="C79" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:25</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>34.19583205457905</v>
+      </c>
+      <c r="C80" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:27</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>43.99497356409945</v>
+      </c>
+      <c r="C81" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:29</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>43.9498463143959</v>
+      </c>
+      <c r="C82" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:31</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>35.75322894977879</v>
+      </c>
+      <c r="C83" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:33</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>34.65542655939027</v>
+      </c>
+      <c r="C84" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:35</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>30.97401210256555</v>
+      </c>
+      <c r="C85" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:37</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>46.38667028515582</v>
+      </c>
+      <c r="C86" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:39</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>37.46711371127068</v>
+      </c>
+      <c r="C87" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:41</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>33.94196487002468</v>
+      </c>
+      <c r="C88" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:43</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>35.64746838334304</v>
+      </c>
+      <c r="C89" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:45</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>34.61488136785064</v>
+      </c>
+      <c r="C90" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:47</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>42.37741692251688</v>
+      </c>
+      <c r="C91" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:49</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>42.53161075686781</v>
+      </c>
+      <c r="C92" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:51</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>39.58328894745962</v>
+      </c>
+      <c r="C93" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:53</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>41.6360849313354</v>
+      </c>
+      <c r="C94" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:55</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>39.81240944202523</v>
+      </c>
+      <c r="C95" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:57</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>39.47969655216603</v>
+      </c>
+      <c r="C96" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:59</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>48.25940329513917</v>
+      </c>
+      <c r="C97" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:01</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>32.02725882868254</v>
+      </c>
+      <c r="C98" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:03</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>36.19769834319804</v>
+      </c>
+      <c r="C99" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:05</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>49.3591435925719</v>
+      </c>
+      <c r="C100" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:07</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>43.62493332316598</v>
+      </c>
+      <c r="C101" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:09</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>46.21920512804258</v>
+      </c>
+      <c r="C102" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:11</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>39.23548599862956</v>
+      </c>
+      <c r="C103" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:13</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>41.93780505571603</v>
+      </c>
+      <c r="C104" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:15</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>46.92297573724627</v>
+      </c>
+      <c r="C105" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:17</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>49.29415536944021</v>
+      </c>
+      <c r="C106" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:19</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>37.14748250797692</v>
+      </c>
+      <c r="C107" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:21</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>36.86755317670647</v>
+      </c>
+      <c r="C108" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:23</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>41.27281576009418</v>
+      </c>
+      <c r="C109" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:25</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>33.95186446528007</v>
+      </c>
+      <c r="C110" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:27</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>36.23310379494188</v>
+      </c>
+      <c r="C111" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:29</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>44.91588586697554</v>
+      </c>
+      <c r="C112" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:31</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>34.87116670294344</v>
+      </c>
+      <c r="C113" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:33</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>42.92431043991477</v>
+      </c>
+      <c r="C114" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:35</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>41.27716291854778</v>
+      </c>
+      <c r="C115" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:37</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>33.23049236488003</v>
+      </c>
+      <c r="C116" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:39</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>38.05710550323509</v>
+      </c>
+      <c r="C117" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:41</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>57.00855475339036</v>
+      </c>
+      <c r="C118" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:43</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>44.54126746937795</v>
+      </c>
+      <c r="C119" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:45</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>34.52921133325363</v>
+      </c>
+      <c r="C120" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:47</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>39.59286035188139</v>
+      </c>
+      <c r="C121" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:49</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>37.09105266942664</v>
+      </c>
+      <c r="C122" t="n">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -852,7 +2035,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -885,7 +2068,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:08</t>
+          <t>2024-08-27 21:28:46</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -895,7 +2078,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>26.27 and 29.66</t>
+          <t>34.24 and 38.61</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -905,7 +2088,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:09</t>
+          <t>2024-08-27 21:28:46</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -915,17 +2098,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>29.56 and 0.00</t>
+          <t>0.00 and 40.44</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:27</t>
+          <t>2024-08-27 21:28:47</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -935,7 +2118,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>38.18 and 43.76</t>
+          <t>0.00 and 83.90</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -945,47 +2128,47 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:30</t>
+          <t>2024-08-27 21:28:51</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.00 and 26.17</t>
+          <t>44.47 and 26.24</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:40</t>
+          <t>2024-08-27 21:28:52</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>31.16 and 41.78</t>
+          <t>29.02 and 30.62</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-27 14:49:41</t>
+          <t>2024-08-27 21:28:58</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -995,11 +2178,1011 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>33.89 and 0.00</t>
+          <t>59.08 and 38.11</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:29:03</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>28.73 and 33.36</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:29:05</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>40.59 and 0.00</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:29:11</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>32.92 and 41.41</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:29:21</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>28.22 and 39.21</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:29:25</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>6.00 and 34.90</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:29:27</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>34.16 and 37.09</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:29:27</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>28.16 and 37.11</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:29:37</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>28.97 and 36.08</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:09</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>34.60 and 81.35</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:09</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>41.86 and 0.00</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:10</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>35.92 and 37.84</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:17</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>80.87 and 29.76</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:18</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>31.82 and 59.57</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0.00 and 37.18</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:20</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>38.98 and 0.00</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:29</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>30.09 and 43.27</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:29</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>28.73 and 41.47</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:31</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>28.69 and 0.00</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:46</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>39.39 and 36.68</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:47</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0.00 and 36.93</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:48</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0.00 and 31.96</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:30:50</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>37.70 and 41.28</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:12</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0.00 and 31.91</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:15</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0.00 and 37.34</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:18</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>38.37 and 82.78</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:20</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2.00 and 41.87</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:23</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>41.13 and 28.76</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:31</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>31.05 and 82.40</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:33</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>33.29 and 39.45</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:34</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>41.11 and 0.00</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:42</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>34.36 and 31.67</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:43</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>84.79 and 0.00</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:31:49</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>42.22 and 32.68</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:00</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>45.54 and 38.33</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:00</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>35.86 and 0.00</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:00</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>84.60 and 43.04</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:11</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>30.10 and 37.09</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:17</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>35.52 and 38.64</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:17</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0.00 and 35.50</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:19</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>33.17 and 45.11</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:20</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>53.87 and 0.00</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:25</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0.00 and 84.12</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:28</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>34.23 and 0.00</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:29</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>42.51 and 40.30</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:29</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>36.25 and 0.00</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:36</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>42.68 and 29.63</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:39</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>38.88 and 0.00</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:44</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>78.90 and 46.41</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:46</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>39.13 and 52.82</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-08-27 21:32:46</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>45.74 and 0.00</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed fovs - but why?
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-28 14:33:59</t>
+          <t>2024-08-28 17:21:18</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>37.76155461340608</v>
+        <v>37.55490894322983</v>
       </c>
       <c r="C2" t="n">
         <v>8</v>
@@ -467,222 +467,157 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:01</t>
+          <t>2024-08-28 17:21:20</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>37.75692097747697</v>
+        <v>36.15062400517214</v>
       </c>
       <c r="C3" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:03</t>
+          <t>2024-08-28 17:21:22</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>40.055154403167</v>
+        <v>35.15737758284577</v>
       </c>
       <c r="C4" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:06</t>
+          <t>2024-08-28 17:21:24</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>48.01005191742476</v>
+        <v>33.27148322901341</v>
       </c>
       <c r="C5" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:08</t>
+          <t>2024-08-28 17:21:26</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>42.42706560910882</v>
+        <v>35.68417963447074</v>
       </c>
       <c r="C6" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:10</t>
+          <t>2024-08-28 17:21:29</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>44.69290495173266</v>
+        <v>34.05210373195279</v>
       </c>
       <c r="C7" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:12</t>
+          <t>2024-08-28 17:21:31</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>34.3775403147386</v>
+        <v>35.11168667382415</v>
       </c>
       <c r="C8" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:14</t>
+          <t>2024-08-28 17:21:33</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>37.10432159197703</v>
+        <v>34.45730914588974</v>
       </c>
       <c r="C9" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:16</t>
+          <t>2024-08-28 17:21:35</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>37.97401576708322</v>
+        <v>30.08983503040512</v>
       </c>
       <c r="C10" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:18</t>
+          <t>2024-08-28 17:21:37</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>32.22511645200283</v>
+        <v>28.57848323067096</v>
       </c>
       <c r="C11" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:20</t>
+          <t>2024-08-28 17:21:39</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>24.09735969052906</v>
+        <v>31.11678594657995</v>
       </c>
       <c r="C12" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:22</t>
+          <t>2024-08-28 17:21:41</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>43.98122939385809</v>
+        <v>28.00793533950663</v>
       </c>
       <c r="C13" t="n">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:24</t>
+          <t>2024-08-28 17:21:43</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>36.45751024131139</v>
+        <v>20.17901844736679</v>
       </c>
       <c r="C14" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2024-08-28 14:34:26</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>29.09669984500469</v>
-      </c>
-      <c r="C15" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2024-08-28 14:34:28</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>34.27848470130493</v>
-      </c>
-      <c r="C16" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2024-08-28 14:34:30</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>39.74022538571077</v>
-      </c>
-      <c r="C17" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2024-08-28 14:34:32</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>35.20326554968279</v>
-      </c>
-      <c r="C18" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2024-08-28 14:34:34</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>25.98701019974309</v>
-      </c>
-      <c r="C19" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -696,7 +631,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -729,17 +664,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:09</t>
+          <t>2024-08-28 17:21:33</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Truck and Car</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>42.22 and 48.59</t>
+          <t>31.04 and 38.58</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -749,17 +684,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:12</t>
+          <t>2024-08-28 17:21:41</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.00 and 36.51</t>
+          <t>35.93 and 37.05</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -769,7 +704,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:13</t>
+          <t>2024-08-28 17:21:42</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -779,7 +714,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>51.18 and 0.00</t>
+          <t>0.00 and 33.31</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -789,7 +724,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-28 14:34:15</t>
+          <t>2024-08-28 17:21:44</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -799,191 +734,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>52.90 and 0.00</t>
+          <t>0.00 and 37.54</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2024-08-28 14:34:17</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>35.64 and 35.32</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2024-08-28 14:34:18</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>30.69 and 84.48</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2024-08-28 14:34:18</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>38.01 and 43.72</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2024-08-28 14:34:19</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>33.84 and 0.00</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2024-08-28 14:34:20</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>37.25 and 0.00</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2024-08-28 14:34:21</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>28.29 and 0.00</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2024-08-28 14:34:23</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Truck and Car</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>31.11 and 78.79</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2024-08-28 14:34:32</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>41.80 and 56.80</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2024-08-28 14:34:33</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>45.83 and 0.00</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kinda working right of way?
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,170 +454,534 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-28 17:21:18</t>
+          <t>2024-08-30 17:46:51</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>37.55490894322983</v>
+        <v>37.77004115973082</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-28 17:21:20</t>
+          <t>2024-08-30 17:46:53</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>36.15062400517214</v>
+        <v>40.73859557846516</v>
       </c>
       <c r="C3" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-28 17:21:22</t>
+          <t>2024-08-30 17:46:55</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>35.15737758284577</v>
+        <v>42.49414241087165</v>
       </c>
       <c r="C4" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-28 17:21:24</t>
+          <t>2024-08-30 17:46:57</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>33.27148322901341</v>
+        <v>41.58947428792983</v>
       </c>
       <c r="C5" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-28 17:21:26</t>
+          <t>2024-08-30 17:46:59</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>35.68417963447074</v>
+        <v>40.83009347718625</v>
       </c>
       <c r="C6" t="n">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-28 17:21:29</t>
+          <t>2024-08-30 17:47:01</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>34.05210373195279</v>
+        <v>38.75166211219071</v>
       </c>
       <c r="C7" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-08-28 17:21:31</t>
+          <t>2024-08-30 17:47:03</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>35.11168667382415</v>
+        <v>32.35722412824396</v>
       </c>
       <c r="C8" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-08-28 17:21:33</t>
+          <t>2024-08-30 17:47:05</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>34.45730914588974</v>
+        <v>26.6200271275341</v>
       </c>
       <c r="C9" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-08-28 17:21:35</t>
+          <t>2024-08-30 17:47:07</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>30.08983503040512</v>
+        <v>26.19534311713419</v>
       </c>
       <c r="C10" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-08-28 17:21:37</t>
+          <t>2024-08-30 17:47:09</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>28.57848323067096</v>
+        <v>24.63855276244706</v>
       </c>
       <c r="C11" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-08-28 17:21:39</t>
+          <t>2024-08-30 17:47:11</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>31.11678594657995</v>
+        <v>19.40124352172453</v>
       </c>
       <c r="C12" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2024-08-28 17:21:41</t>
+          <t>2024-08-30 17:47:13</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>28.00793533950663</v>
+        <v>20.73606382158988</v>
       </c>
       <c r="C13" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2024-08-28 17:21:43</t>
+          <t>2024-08-30 17:47:15</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>20.17901844736679</v>
+        <v>22.56519589868218</v>
       </c>
       <c r="C14" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:17</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>19.38998777883178</v>
+      </c>
+      <c r="C15" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:19</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>16.63371161896305</v>
+      </c>
+      <c r="C16" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:21</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>16.45943976444216</v>
+      </c>
+      <c r="C17" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:23</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>12.27585630456286</v>
+      </c>
+      <c r="C18" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:25</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>14.20376145335394</v>
+      </c>
+      <c r="C19" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:27</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>13.94596721012559</v>
+      </c>
+      <c r="C20" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:29</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>13.53278244398157</v>
+      </c>
+      <c r="C21" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:31</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>10.6247001290159</v>
+      </c>
+      <c r="C22" t="n">
         <v>38</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:33</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>12.77179836720124</v>
+      </c>
+      <c r="C23" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:35</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>8.126224276215465</v>
+      </c>
+      <c r="C24" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:37</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>11.7039561148478</v>
+      </c>
+      <c r="C25" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:39</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>12.69294224291906</v>
+      </c>
+      <c r="C26" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:41</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>12.21244462341455</v>
+      </c>
+      <c r="C27" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:43</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>12.40883255124898</v>
+      </c>
+      <c r="C28" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:45</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>12.35205869896399</v>
+      </c>
+      <c r="C29" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:47</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>16.30887470148119</v>
+      </c>
+      <c r="C30" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:49</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>15.07645122862061</v>
+      </c>
+      <c r="C31" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:51</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>14.70820794473461</v>
+      </c>
+      <c r="C32" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:53</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>15.79663702859301</v>
+      </c>
+      <c r="C33" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:55</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>15.47986472960563</v>
+      </c>
+      <c r="C34" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:57</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>14.21622389460384</v>
+      </c>
+      <c r="C35" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:47:59</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>11.26183079164776</v>
+      </c>
+      <c r="C36" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:48:01</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>13.19390537128629</v>
+      </c>
+      <c r="C37" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:48:03</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>9.157998235261848</v>
+      </c>
+      <c r="C38" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:48:05</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>7.42380171494699</v>
+      </c>
+      <c r="C39" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:48:07</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>7.227210829806319</v>
+      </c>
+      <c r="C40" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:48:09</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>4.207789989153946</v>
+      </c>
+      <c r="C41" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-08-30 17:48:11</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>2.969678404867152</v>
+      </c>
+      <c r="C42" t="n">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -631,7 +995,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -664,81 +1028,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-28 17:21:33</t>
+          <t>2024-08-30 17:47:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Truck and Car</t>
+          <t>Car and Car</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>31.04 and 38.58</t>
+          <t>28.76 and 23.27</t>
         </is>
       </c>
       <c r="D2" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-08-28 17:21:41</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Car and Truck</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>35.93 and 37.05</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-08-28 17:21:42</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.00 and 33.31</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-08-28 17:21:44</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.00 and 37.54</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding queue to junction
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-30 17:46:51</t>
+          <t>2024-08-30 21:16:03</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>37.77004115973082</v>
+        <v>33.36845952394092</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
@@ -467,11 +467,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-30 17:46:53</t>
+          <t>2024-08-30 21:16:05</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>40.73859557846516</v>
+        <v>36.18499795343281</v>
       </c>
       <c r="C3" t="n">
         <v>8</v>
@@ -480,37 +480,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-30 17:46:55</t>
+          <t>2024-08-30 21:16:07</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>42.49414241087165</v>
+        <v>38.13729141410148</v>
       </c>
       <c r="C4" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-30 17:46:57</t>
+          <t>2024-08-30 21:16:09</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>41.58947428792983</v>
+        <v>38.54517290604009</v>
       </c>
       <c r="C5" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-30 17:46:59</t>
+          <t>2024-08-30 21:16:11</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>40.83009347718625</v>
+        <v>40.10152733482884</v>
       </c>
       <c r="C6" t="n">
         <v>17</v>
@@ -519,37 +519,37 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:01</t>
+          <t>2024-08-30 21:16:14</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>38.75166211219071</v>
+        <v>37.83928087094589</v>
       </c>
       <c r="C7" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:03</t>
+          <t>2024-08-30 21:16:16</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>32.35722412824396</v>
+        <v>33.64837695736625</v>
       </c>
       <c r="C8" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:05</t>
+          <t>2024-08-30 21:16:18</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>26.6200271275341</v>
+        <v>33.91395395140444</v>
       </c>
       <c r="C9" t="n">
         <v>26</v>
@@ -558,141 +558,141 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:07</t>
+          <t>2024-08-30 21:16:20</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>26.19534311713419</v>
+        <v>28.2301595680891</v>
       </c>
       <c r="C10" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:09</t>
+          <t>2024-08-30 21:16:22</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>24.63855276244706</v>
+        <v>29.85904993760463</v>
       </c>
       <c r="C11" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:11</t>
+          <t>2024-08-30 21:16:24</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>19.40124352172453</v>
+        <v>29.5493732380974</v>
       </c>
       <c r="C12" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:13</t>
+          <t>2024-08-30 21:16:26</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>20.73606382158988</v>
+        <v>27.00575810892638</v>
       </c>
       <c r="C13" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:15</t>
+          <t>2024-08-30 21:16:28</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>22.56519589868218</v>
+        <v>25.19415498944947</v>
       </c>
       <c r="C14" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:17</t>
+          <t>2024-08-30 21:16:30</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>19.38998777883178</v>
+        <v>23.83743746686357</v>
       </c>
       <c r="C15" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:19</t>
+          <t>2024-08-30 21:16:32</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>16.63371161896305</v>
+        <v>22.58287766971266</v>
       </c>
       <c r="C16" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:21</t>
+          <t>2024-08-30 21:16:34</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>16.45943976444216</v>
+        <v>21.42318548347823</v>
       </c>
       <c r="C17" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:23</t>
+          <t>2024-08-30 21:17:12</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>12.27585630456286</v>
+        <v>19.97962162743501</v>
       </c>
       <c r="C18" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:25</t>
+          <t>2024-08-30 21:17:14</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>14.20376145335394</v>
+        <v>16.73296032689855</v>
       </c>
       <c r="C19" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:27</t>
+          <t>2024-08-30 21:17:16</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>13.94596721012559</v>
+        <v>17.88842700428664</v>
       </c>
       <c r="C20" t="n">
         <v>41</v>
@@ -701,11 +701,11 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:29</t>
+          <t>2024-08-30 21:17:18</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>13.53278244398157</v>
+        <v>19.44136268782263</v>
       </c>
       <c r="C21" t="n">
         <v>40</v>
@@ -714,76 +714,76 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:31</t>
+          <t>2024-08-30 21:17:20</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>10.6247001290159</v>
+        <v>17.24289317434194</v>
       </c>
       <c r="C22" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:33</t>
+          <t>2024-08-30 21:17:22</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>12.77179836720124</v>
+        <v>17.4161599985886</v>
       </c>
       <c r="C23" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:35</t>
+          <t>2024-08-30 21:17:24</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>8.126224276215465</v>
+        <v>15.91116227216883</v>
       </c>
       <c r="C24" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:37</t>
+          <t>2024-08-30 21:17:26</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>11.7039561148478</v>
+        <v>16.3350609746136</v>
       </c>
       <c r="C25" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:39</t>
+          <t>2024-08-30 21:17:28</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>12.69294224291906</v>
+        <v>17.51482579951818</v>
       </c>
       <c r="C26" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:41</t>
+          <t>2024-08-30 21:17:30</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>12.21244462341455</v>
+        <v>17.20392362997698</v>
       </c>
       <c r="C27" t="n">
         <v>38</v>
@@ -792,196 +792,118 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:43</t>
+          <t>2024-08-30 21:17:32</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>12.40883255124898</v>
+        <v>17.81991207315941</v>
       </c>
       <c r="C28" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:45</t>
+          <t>2024-08-30 21:17:34</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>12.35205869896399</v>
+        <v>15.91981948055395</v>
       </c>
       <c r="C29" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:47</t>
+          <t>2024-08-30 21:17:36</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>16.30887470148119</v>
+        <v>14.49940314875241</v>
       </c>
       <c r="C30" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:49</t>
+          <t>2024-08-30 21:17:38</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>15.07645122862061</v>
+        <v>15.5213523136577</v>
       </c>
       <c r="C31" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:51</t>
+          <t>2024-08-30 21:17:40</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>14.70820794473461</v>
+        <v>17.98013377150679</v>
       </c>
       <c r="C32" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:53</t>
+          <t>2024-08-30 21:17:42</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>15.79663702859301</v>
+        <v>17.70205052664934</v>
       </c>
       <c r="C33" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:55</t>
+          <t>2024-08-30 21:17:44</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>15.47986472960563</v>
+        <v>17.85047680230193</v>
       </c>
       <c r="C34" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:57</t>
+          <t>2024-08-30 21:17:46</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>14.21622389460384</v>
+        <v>15.19020394449197</v>
       </c>
       <c r="C35" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:59</t>
+          <t>2024-08-30 21:17:48</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>11.26183079164776</v>
+        <v>15.25731561172521</v>
       </c>
       <c r="C36" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>2024-08-30 17:48:01</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>13.19390537128629</v>
-      </c>
-      <c r="C37" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>2024-08-30 17:48:03</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>9.157998235261848</v>
-      </c>
-      <c r="C38" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>2024-08-30 17:48:05</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>7.42380171494699</v>
-      </c>
-      <c r="C39" t="n">
         <v>40</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>2024-08-30 17:48:07</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>7.227210829806319</v>
-      </c>
-      <c r="C40" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>2024-08-30 17:48:09</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>4.207789989153946</v>
-      </c>
-      <c r="C41" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>2024-08-30 17:48:11</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>2.969678404867152</v>
-      </c>
-      <c r="C42" t="n">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -995,7 +917,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1028,20 +950,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-30 17:47:34</t>
+          <t>2024-08-30 21:16:32</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Car and Car</t>
+          <t>Car and Truck</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>28.76 and 23.27</t>
+          <t>28.77 and 20.30</t>
         </is>
       </c>
       <c r="D2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-08-30 21:16:34</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Car and Truck</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>29.10 and 0.00</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
continued working on right of way
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-30 21:16:03</t>
+          <t>2024-08-31 17:53:24</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>33.36845952394092</v>
+        <v>46.23207377094948</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
@@ -467,50 +467,50 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-08-30 21:16:05</t>
+          <t>2024-08-31 17:53:26</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>36.18499795343281</v>
+        <v>45.44482058155278</v>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-08-30 21:16:07</t>
+          <t>2024-08-31 17:53:28</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>38.13729141410148</v>
+        <v>43.5787008554075</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-08-30 21:16:09</t>
+          <t>2024-08-31 17:53:30</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>38.54517290604009</v>
+        <v>43.07859483232566</v>
       </c>
       <c r="C5" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-30 21:16:11</t>
+          <t>2024-08-31 17:53:32</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>40.10152733482884</v>
+        <v>39.92638354542284</v>
       </c>
       <c r="C6" t="n">
         <v>17</v>
@@ -519,391 +519,14 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-08-30 21:16:14</t>
+          <t>2024-08-31 17:53:34</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>37.83928087094589</v>
+        <v>38.03167310516027</v>
       </c>
       <c r="C7" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:16:16</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>33.64837695736625</v>
-      </c>
-      <c r="C8" t="n">
         <v>21</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:16:18</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>33.91395395140444</v>
-      </c>
-      <c r="C9" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:16:20</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>28.2301595680891</v>
-      </c>
-      <c r="C10" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:16:22</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>29.85904993760463</v>
-      </c>
-      <c r="C11" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:16:24</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>29.5493732380974</v>
-      </c>
-      <c r="C12" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:16:26</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>27.00575810892638</v>
-      </c>
-      <c r="C13" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:16:28</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>25.19415498944947</v>
-      </c>
-      <c r="C14" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:16:30</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>23.83743746686357</v>
-      </c>
-      <c r="C15" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:16:32</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>22.58287766971266</v>
-      </c>
-      <c r="C16" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:16:34</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>21.42318548347823</v>
-      </c>
-      <c r="C17" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:12</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>19.97962162743501</v>
-      </c>
-      <c r="C18" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:14</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>16.73296032689855</v>
-      </c>
-      <c r="C19" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:16</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>17.88842700428664</v>
-      </c>
-      <c r="C20" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:18</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>19.44136268782263</v>
-      </c>
-      <c r="C21" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:20</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>17.24289317434194</v>
-      </c>
-      <c r="C22" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:22</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>17.4161599985886</v>
-      </c>
-      <c r="C23" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:24</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>15.91116227216883</v>
-      </c>
-      <c r="C24" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:26</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>16.3350609746136</v>
-      </c>
-      <c r="C25" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:28</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>17.51482579951818</v>
-      </c>
-      <c r="C26" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:30</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>17.20392362997698</v>
-      </c>
-      <c r="C27" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:32</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>17.81991207315941</v>
-      </c>
-      <c r="C28" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:34</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>15.91981948055395</v>
-      </c>
-      <c r="C29" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:36</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>14.49940314875241</v>
-      </c>
-      <c r="C30" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:38</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>15.5213523136577</v>
-      </c>
-      <c r="C31" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:40</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>17.98013377150679</v>
-      </c>
-      <c r="C32" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:42</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>17.70205052664934</v>
-      </c>
-      <c r="C33" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:44</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>17.85047680230193</v>
-      </c>
-      <c r="C34" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:46</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>15.19020394449197</v>
-      </c>
-      <c r="C35" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:17:48</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>15.25731561172521</v>
-      </c>
-      <c r="C36" t="n">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -917,7 +540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -947,46 +570,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:16:32</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Car and Truck</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>28.77 and 20.30</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-08-30 21:16:34</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Car and Truck</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>29.10 and 0.00</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
working right of way???
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,83 +450,34 @@
           <t>Density</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 0, Direction 0)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 0, Direction 1)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-31 17:53:24</t>
+          <t>2024-08-31 21:58:14</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>46.23207377094948</v>
+        <v>45.48956516402566</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-08-31 17:53:26</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>45.44482058155278</v>
-      </c>
-      <c r="C3" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-08-31 17:53:28</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>43.5787008554075</v>
-      </c>
-      <c r="C4" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-08-31 17:53:30</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>43.07859483232566</v>
-      </c>
-      <c r="C5" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2024-08-31 17:53:32</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>39.92638354542284</v>
-      </c>
-      <c r="C6" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2024-08-31 17:53:34</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>38.03167310516027</v>
-      </c>
-      <c r="C7" t="n">
-        <v>21</v>
+        <v>4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>45.38705485689707</v>
+      </c>
+      <c r="E2" t="n">
+        <v>45.59207547115425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated pictures and minor changes to vehicle
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,24 +460,48 @@
           <t>Avg. Speed (Road 0, Direction 1)</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 1, Direction 0)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 1, Direction 1)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 2, Direction 0)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-31 21:58:14</t>
+          <t>2024-09-01 16:16:28</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>45.48956516402566</v>
+        <v>43.24172181965915</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>45.38705485689707</v>
+        <v>42.80508055616068</v>
       </c>
       <c r="E2" t="n">
-        <v>45.59207547115425</v>
+        <v>45.71323319191159</v>
+      </c>
+      <c r="F2" t="n">
+        <v>37.69324910085565</v>
+      </c>
+      <c r="G2" t="n">
+        <v>41.47129424928515</v>
+      </c>
+      <c r="H2" t="n">
+        <v>48.52575200008273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working roundabout still not right of way
</commit_message>
<xml_diff>
--- a/simulation_data.xlsx
+++ b/simulation_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,25 +460,630 @@
           <t>Avg. Speed (Road 0, Direction 1)</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 1, Direction 0)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 1, Direction 1)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 2, Direction 0)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 2, Direction 1)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-31 21:58:14</t>
+          <t>2024-09-02 23:12:49</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>45.48956516402566</v>
+        <v>39.32999301634911</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>45.38705485689707</v>
+        <v>32.16814285696761</v>
       </c>
       <c r="E2" t="n">
-        <v>45.59207547115425</v>
-      </c>
+        <v>52.39009862729739</v>
+      </c>
+      <c r="F2" t="n">
+        <v>40.92742988535939</v>
+      </c>
+      <c r="G2" t="n">
+        <v>43.6879705382381</v>
+      </c>
+      <c r="H2" t="n">
+        <v>27.47632317388308</v>
+      </c>
+      <c r="I2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:12:51</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>40.26300741434243</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" t="n">
+        <v>42.61619386209097</v>
+      </c>
+      <c r="E3" t="n">
+        <v>51.09251957846763</v>
+      </c>
+      <c r="F3" t="n">
+        <v>24.55645793121563</v>
+      </c>
+      <c r="G3" t="n">
+        <v>41.32692566426174</v>
+      </c>
+      <c r="H3" t="n">
+        <v>27.47632317388308</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:14:48</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>40.36197050294333</v>
+      </c>
+      <c r="C4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" t="n">
+        <v>38.10253720250196</v>
+      </c>
+      <c r="E4" t="n">
+        <v>51.25578070281274</v>
+      </c>
+      <c r="F4" t="n">
+        <v>34.13314930062516</v>
+      </c>
+      <c r="G4" t="n">
+        <v>41.428096551815</v>
+      </c>
+      <c r="H4" t="n">
+        <v>36.8902887569618</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:14:50</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>38.42515922773548</v>
+      </c>
+      <c r="C5" t="n">
+        <v>14</v>
+      </c>
+      <c r="D5" t="n">
+        <v>25.03308156949241</v>
+      </c>
+      <c r="E5" t="n">
+        <v>47.72943049756515</v>
+      </c>
+      <c r="F5" t="n">
+        <v>25.28703240233679</v>
+      </c>
+      <c r="G5" t="n">
+        <v>43.14286038643494</v>
+      </c>
+      <c r="H5" t="n">
+        <v>39.67107318192354</v>
+      </c>
+      <c r="I5" t="n">
+        <v>45.68190904686756</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:14:55</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>39.42549235476026</v>
+      </c>
+      <c r="C6" t="n">
+        <v>14</v>
+      </c>
+      <c r="D6" t="n">
+        <v>38.02356636931299</v>
+      </c>
+      <c r="E6" t="n">
+        <v>47.72943049756515</v>
+      </c>
+      <c r="F6" t="n">
+        <v>25.28293008931708</v>
+      </c>
+      <c r="G6" t="n">
+        <v>41.63881375616702</v>
+      </c>
+      <c r="H6" t="n">
+        <v>37.18575274710647</v>
+      </c>
+      <c r="I6" t="n">
+        <v>45.68190904686756</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:14:57</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>38.1487681653112</v>
+      </c>
+      <c r="C7" t="n">
+        <v>17</v>
+      </c>
+      <c r="D7" t="n">
+        <v>38.90957394637607</v>
+      </c>
+      <c r="E7" t="n">
+        <v>44.04977636682329</v>
+      </c>
+      <c r="F7" t="n">
+        <v>32.51756079950753</v>
+      </c>
+      <c r="G7" t="n">
+        <v>35.86932030967526</v>
+      </c>
+      <c r="H7" t="n">
+        <v>33.10466049349071</v>
+      </c>
+      <c r="I7" t="n">
+        <v>45.0180903211123</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:14:59</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>35.50323949003175</v>
+      </c>
+      <c r="C8" t="n">
+        <v>19</v>
+      </c>
+      <c r="D8" t="n">
+        <v>34.20309540763891</v>
+      </c>
+      <c r="E8" t="n">
+        <v>43.79970258176093</v>
+      </c>
+      <c r="F8" t="n">
+        <v>26.16662815598896</v>
+      </c>
+      <c r="G8" t="n">
+        <v>31.33206487404325</v>
+      </c>
+      <c r="H8" t="n">
+        <v>34.26643567780569</v>
+      </c>
+      <c r="I8" t="n">
+        <v>45.03133124645953</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:02</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>36.56230278532624</v>
+      </c>
+      <c r="C9" t="n">
+        <v>23</v>
+      </c>
+      <c r="D9" t="n">
+        <v>35.60614600605002</v>
+      </c>
+      <c r="E9" t="n">
+        <v>43.4870464962688</v>
+      </c>
+      <c r="F9" t="n">
+        <v>31.44995545715049</v>
+      </c>
+      <c r="G9" t="n">
+        <v>30.29224623742075</v>
+      </c>
+      <c r="H9" t="n">
+        <v>35.92502029435428</v>
+      </c>
+      <c r="I9" t="n">
+        <v>45.04269265647653</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:04</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>33.9114820392279</v>
+      </c>
+      <c r="C10" t="n">
+        <v>25</v>
+      </c>
+      <c r="D10" t="n">
+        <v>23.02764075893078</v>
+      </c>
+      <c r="E10" t="n">
+        <v>42.88780986488958</v>
+      </c>
+      <c r="F10" t="n">
+        <v>26.66370028889645</v>
+      </c>
+      <c r="G10" t="n">
+        <v>28.36958859434387</v>
+      </c>
+      <c r="H10" t="n">
+        <v>35.23985555420444</v>
+      </c>
+      <c r="I10" t="n">
+        <v>44.74036988190556</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:06</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>27.40177790417046</v>
+      </c>
+      <c r="C11" t="n">
+        <v>27</v>
+      </c>
+      <c r="D11" t="n">
+        <v>18.17616745263575</v>
+      </c>
+      <c r="E11" t="n">
+        <v>30.17531444981829</v>
+      </c>
+      <c r="F11" t="n">
+        <v>22.40075175675853</v>
+      </c>
+      <c r="G11" t="n">
+        <v>21.37505085054659</v>
+      </c>
+      <c r="H11" t="n">
+        <v>32.21228928997608</v>
+      </c>
+      <c r="I11" t="n">
+        <v>44.45799109074632</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:08</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>24.4147090962771</v>
+      </c>
+      <c r="C12" t="n">
+        <v>29</v>
+      </c>
+      <c r="D12" t="n">
+        <v>7.378489326644028</v>
+      </c>
+      <c r="E12" t="n">
+        <v>27.79528595594022</v>
+      </c>
+      <c r="F12" t="n">
+        <v>17.32116194912201</v>
+      </c>
+      <c r="G12" t="n">
+        <v>23.44971991988833</v>
+      </c>
+      <c r="H12" t="n">
+        <v>23.55144745979688</v>
+      </c>
+      <c r="I12" t="n">
+        <v>44.81177848649895</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:10</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>22.51667623913327</v>
+      </c>
+      <c r="C13" t="n">
+        <v>32</v>
+      </c>
+      <c r="D13" t="n">
+        <v>31.96746152663822</v>
+      </c>
+      <c r="E13" t="n">
+        <v>29.45134653620259</v>
+      </c>
+      <c r="F13" t="n">
+        <v>15.36134461861789</v>
+      </c>
+      <c r="G13" t="n">
+        <v>15.03904849801967</v>
+      </c>
+      <c r="H13" t="n">
+        <v>18.7754417751161</v>
+      </c>
+      <c r="I13" t="n">
+        <v>44.80116484763707</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:12</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>17.09135074446053</v>
+      </c>
+      <c r="C14" t="n">
+        <v>33</v>
+      </c>
+      <c r="D14" t="n">
+        <v>12.52017418229494</v>
+      </c>
+      <c r="E14" t="n">
+        <v>23.63094328358969</v>
+      </c>
+      <c r="F14" t="n">
+        <v>10.09841163540567</v>
+      </c>
+      <c r="G14" t="n">
+        <v>13.45888408351396</v>
+      </c>
+      <c r="H14" t="n">
+        <v>14.5842669151818</v>
+      </c>
+      <c r="I14" t="n">
+        <v>44.78032765834941</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:14</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>18.67466579403028</v>
+      </c>
+      <c r="C15" t="n">
+        <v>34</v>
+      </c>
+      <c r="D15" t="n">
+        <v>21.72674216564357</v>
+      </c>
+      <c r="E15" t="n">
+        <v>25.37696809951719</v>
+      </c>
+      <c r="F15" t="n">
+        <v>8.434339738122286</v>
+      </c>
+      <c r="G15" t="n">
+        <v>12.46877480464703</v>
+      </c>
+      <c r="H15" t="n">
+        <v>16.9325950190036</v>
+      </c>
+      <c r="I15" t="n">
+        <v>44.6800042120723</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:16</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>14.91127966264332</v>
+      </c>
+      <c r="C16" t="n">
+        <v>36</v>
+      </c>
+      <c r="D16" t="n">
+        <v>19.18936246426791</v>
+      </c>
+      <c r="E16" t="n">
+        <v>21.48793361561635</v>
+      </c>
+      <c r="F16" t="n">
+        <v>21.15197017229543</v>
+      </c>
+      <c r="G16" t="n">
+        <v>5.57089029545177</v>
+      </c>
+      <c r="H16" t="n">
+        <v>6.140373817786553</v>
+      </c>
+      <c r="I16" t="n">
+        <v>46.05528151786155</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:18</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>12.78712289329854</v>
+      </c>
+      <c r="C17" t="n">
+        <v>37</v>
+      </c>
+      <c r="D17" t="n">
+        <v>14.14264850072641</v>
+      </c>
+      <c r="E17" t="n">
+        <v>22.5662127614318</v>
+      </c>
+      <c r="F17" t="n">
+        <v>16.96166406291684</v>
+      </c>
+      <c r="G17" t="n">
+        <v>7.147348691189086</v>
+      </c>
+      <c r="H17" t="n">
+        <v>6.198275539861843</v>
+      </c>
+      <c r="I17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:20</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>10.19735743114137</v>
+      </c>
+      <c r="C18" t="n">
+        <v>39</v>
+      </c>
+      <c r="D18" t="n">
+        <v>6.19071576499829</v>
+      </c>
+      <c r="E18" t="n">
+        <v>23.94694977066507</v>
+      </c>
+      <c r="F18" t="n">
+        <v>12.79214925286104</v>
+      </c>
+      <c r="G18" t="n">
+        <v>4.715913046818263</v>
+      </c>
+      <c r="H18" t="n">
+        <v>3.202470011500567</v>
+      </c>
+      <c r="I18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:22</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>10.43689971875165</v>
+      </c>
+      <c r="C19" t="n">
+        <v>38</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>29.37626428811924</v>
+      </c>
+      <c r="F19" t="n">
+        <v>20.97084762164731</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3.738499899184171</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2.775825457400244</v>
+      </c>
+      <c r="I19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:24</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>5.368947563381441</v>
+      </c>
+      <c r="C20" t="n">
+        <v>39</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>19.82149262027967</v>
+      </c>
+      <c r="F20" t="n">
+        <v>6.258179277415345</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.9810064253857803</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.3457874091288957</v>
+      </c>
+      <c r="I20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:26</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>10.63178307816429</v>
+      </c>
+      <c r="C21" t="n">
+        <v>40</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>33.75975973350439</v>
+      </c>
+      <c r="F21" t="n">
+        <v>18.0292720068903</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3.997822347692966</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.3041567392571939</v>
+      </c>
+      <c r="I21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -491,7 +1096,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,6 +1126,66 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:12</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>3.09 and 37.44</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:17</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Car and Car</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>18.99 and 25.02</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-09-02 23:15:21</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Truck and Car</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>28.21 and 29.17</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>